<commit_message>
changes to data and changes to reply to reviewers
</commit_message>
<xml_diff>
--- a/data/AllData_Catchments.xlsx
+++ b/data/AllData_Catchments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC09B5F9-812A-47AF-BD3F-C68B98ECC176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C082251D-7125-4254-9741-4E6504B50036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
@@ -2173,9 +2173,6 @@
     <t>Swartboskloof</t>
   </si>
   <si>
-    <t>This is Ruprecht and Schofield (1989)</t>
-  </si>
-  <si>
     <t>Ruprecht and Schofield, 1989</t>
   </si>
   <si>
@@ -2490,6 +2487,9 @@
   </si>
   <si>
     <t>Completed 1, Incomplete 0</t>
+  </si>
+  <si>
+    <t>This is Ruprecht and Schofield (1989) rather than Ruprecht and Schofield (1991). Additionally Delta_Forest changed to -100% as the original paper clearly indicates "clearfelling"</t>
   </si>
 </sst>
 </file>
@@ -3189,10 +3189,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="37" t="s">
+        <v>779</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>780</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>781</v>
       </c>
       <c r="I1" s="37" t="s">
         <v>543</v>
@@ -3207,7 +3207,7 @@
         <v>473</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N1" s="37" t="s">
         <v>471</v>
@@ -3222,16 +3222,16 @@
         <v>542</v>
       </c>
       <c r="R1" s="38" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="S1" s="38" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="T1" s="37" t="s">
         <v>624</v>
       </c>
       <c r="U1" s="39" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
@@ -3294,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="28" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
@@ -6995,7 +6995,7 @@
     </row>
     <row r="63" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
   </sheetData>
@@ -7010,14 +7010,16 @@
   <dimension ref="A1:V252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="A1:U252"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="15.59765625" style="2" customWidth="1"/>
-    <col min="3" max="11" width="15.59765625" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.53125" style="2" customWidth="1"/>
+    <col min="3" max="10" width="15.59765625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.53125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.59765625" style="16" customWidth="1"/>
     <col min="13" max="14" width="15.59765625" style="10" customWidth="1"/>
     <col min="15" max="17" width="15.59765625" style="2" customWidth="1"/>
@@ -7049,10 +7051,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="36" t="s">
+        <v>779</v>
+      </c>
+      <c r="H1" s="36" t="s">
         <v>780</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>781</v>
       </c>
       <c r="I1" s="36" t="s">
         <v>543</v>
@@ -7067,7 +7069,7 @@
         <v>473</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N1" s="36" t="s">
         <v>471</v>
@@ -7082,16 +7084,16 @@
         <v>542</v>
       </c>
       <c r="R1" s="38" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="S1" s="37" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="T1" s="37" t="s">
         <v>624</v>
       </c>
       <c r="U1" s="36" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="V1" s="31"/>
     </row>
@@ -7156,7 +7158,7 @@
       </c>
       <c r="T2" s="16"/>
       <c r="U2" s="34" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="V2" s="32"/>
     </row>
@@ -7221,7 +7223,7 @@
       </c>
       <c r="T3" s="16"/>
       <c r="U3" s="34" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="V3" s="32"/>
     </row>
@@ -7432,7 +7434,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="H7" s="6">
         <v>167.7</v>
@@ -7444,7 +7446,7 @@
         <v>12</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="L7" s="49">
         <v>1967</v>
@@ -7472,7 +7474,7 @@
       </c>
       <c r="T7" s="16"/>
       <c r="U7" s="34" t="s">
-        <v>696</v>
+        <v>798</v>
       </c>
       <c r="V7" s="32"/>
     </row>
@@ -7851,7 +7853,7 @@
       </c>
       <c r="T13" s="16"/>
       <c r="U13" s="34" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8041,7 +8043,7 @@
       </c>
       <c r="T16" s="16"/>
       <c r="U16" s="34" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8921,7 +8923,7 @@
         <v>1984</v>
       </c>
       <c r="R30" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S30" s="16">
         <v>1</v>
@@ -9672,7 +9674,7 @@
       </c>
       <c r="T42" s="16"/>
       <c r="U42" s="34" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -9988,7 +9990,7 @@
       </c>
       <c r="T47" s="16"/>
       <c r="U47" s="34" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10300,7 +10302,7 @@
         <v>1964</v>
       </c>
       <c r="R52" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S52" s="16">
         <v>1</v>
@@ -10371,7 +10373,7 @@
       </c>
       <c r="T53" s="16"/>
       <c r="U53" s="34" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="54" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10470,7 +10472,7 @@
         <v>12</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="L55" s="16">
         <v>1263</v>
@@ -10498,7 +10500,7 @@
       </c>
       <c r="T55" s="16"/>
       <c r="U55" s="34" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="56" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10533,7 +10535,7 @@
         <v>12</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="L56" s="16">
         <v>1306</v>
@@ -10561,7 +10563,7 @@
       </c>
       <c r="T56" s="16"/>
       <c r="U56" s="34" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="57" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10812,7 +10814,7 @@
       </c>
       <c r="T60" s="16"/>
       <c r="U60" s="6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -11437,7 +11439,7 @@
       </c>
       <c r="T70" s="16"/>
       <c r="U70" s="34" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12057,7 +12059,7 @@
         <v>1</v>
       </c>
       <c r="U80" s="34" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="81" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14121,7 +14123,7 @@
         <v>12</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="L113" s="16">
         <v>1217</v>
@@ -14147,7 +14149,7 @@
       </c>
       <c r="T113" s="16"/>
       <c r="U113" s="34" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="114" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14243,7 +14245,7 @@
         <v>12</v>
       </c>
       <c r="K115" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="L115" s="16">
         <v>1217</v>
@@ -14272,7 +14274,7 @@
       </c>
       <c r="T115" s="16"/>
       <c r="U115" s="34" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="V115" s="32"/>
     </row>
@@ -14308,7 +14310,7 @@
         <v>12</v>
       </c>
       <c r="K116" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="L116" s="16">
         <v>1217</v>
@@ -14337,7 +14339,7 @@
       </c>
       <c r="T116" s="16"/>
       <c r="U116" s="34" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="117" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14890,7 +14892,7 @@
       </c>
       <c r="T125" s="16"/>
       <c r="U125" s="34" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="V125" s="32"/>
     </row>
@@ -15135,7 +15137,7 @@
         <v>1</v>
       </c>
       <c r="U129" s="34" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="V129" s="32"/>
     </row>
@@ -15393,7 +15395,7 @@
         <v>194</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C134" s="6">
         <v>0.65</v>
@@ -15449,7 +15451,7 @@
       </c>
       <c r="T134" s="16"/>
       <c r="U134" s="34" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="135" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15512,7 +15514,7 @@
       </c>
       <c r="T135" s="16"/>
       <c r="U135" s="34" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="136" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15575,7 +15577,7 @@
       </c>
       <c r="T136" s="16"/>
       <c r="U136" s="34" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="137" spans="1:22" s="13" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15742,7 +15744,7 @@
         <v>1990</v>
       </c>
       <c r="R139" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S139" s="16">
         <v>1</v>
@@ -15993,7 +15995,7 @@
       </c>
       <c r="T143" s="16"/>
       <c r="U143" s="34" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="144" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -16242,7 +16244,7 @@
       </c>
       <c r="T147" s="16"/>
       <c r="U147" s="34" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="148" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -16305,7 +16307,7 @@
       </c>
       <c r="T148" s="16"/>
       <c r="U148" s="34" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="149" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17051,7 +17053,7 @@
         <v>1</v>
       </c>
       <c r="U160" s="34" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="161" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17340,7 +17342,7 @@
         <v>12</v>
       </c>
       <c r="K165" s="6" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="L165" s="16">
         <v>2701</v>
@@ -17366,7 +17368,7 @@
       </c>
       <c r="T165" s="16"/>
       <c r="U165" s="34" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="V165" s="32"/>
     </row>
@@ -17375,7 +17377,7 @@
         <v>225</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C166" s="6">
         <v>0.05</v>
@@ -17402,7 +17404,7 @@
         <v>12</v>
       </c>
       <c r="K166" s="6" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="L166" s="16">
         <v>2701</v>
@@ -17430,7 +17432,7 @@
       </c>
       <c r="T166" s="16"/>
       <c r="U166" s="34" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="167" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17778,7 +17780,7 @@
         <v>12</v>
       </c>
       <c r="K172" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="L172" s="16">
         <v>1491</v>
@@ -17806,7 +17808,7 @@
       </c>
       <c r="T172" s="16"/>
       <c r="U172" s="34" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="173" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17841,7 +17843,7 @@
         <v>12</v>
       </c>
       <c r="K173" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="L173" s="16">
         <v>1429</v>
@@ -17863,7 +17865,7 @@
         <v>1983</v>
       </c>
       <c r="R173" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S173" s="16">
         <v>1</v>
@@ -17905,7 +17907,7 @@
         <v>12</v>
       </c>
       <c r="K174" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="L174" s="16">
         <v>1429</v>
@@ -17927,7 +17929,7 @@
         <v>1983</v>
       </c>
       <c r="R174" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S174" s="16">
         <v>1</v>
@@ -17969,7 +17971,7 @@
         <v>12</v>
       </c>
       <c r="K175" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="L175" s="16">
         <v>1429</v>
@@ -17991,7 +17993,7 @@
         <v>1983</v>
       </c>
       <c r="R175" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S175" s="16">
         <v>1</v>
@@ -18094,7 +18096,7 @@
         <v>12</v>
       </c>
       <c r="K177" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="L177" s="16">
         <v>1429</v>
@@ -18116,7 +18118,7 @@
         <v>1983</v>
       </c>
       <c r="R177" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S177" s="16">
         <v>1</v>
@@ -18158,7 +18160,7 @@
         <v>12</v>
       </c>
       <c r="K178" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="L178" s="16">
         <v>1491</v>
@@ -18186,7 +18188,7 @@
       </c>
       <c r="T178" s="16"/>
       <c r="U178" s="34" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="179" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19245,7 +19247,7 @@
       </c>
       <c r="T195" s="16"/>
       <c r="U195" s="34" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="196" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19301,7 +19303,7 @@
         <v>1990</v>
       </c>
       <c r="R196" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S196" s="16">
         <v>1</v>
@@ -19364,7 +19366,7 @@
         <v>1990</v>
       </c>
       <c r="R197" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S197" s="16">
         <v>1</v>
@@ -19563,7 +19565,7 @@
         <v>0</v>
       </c>
       <c r="U200" s="34" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="201" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20002,7 +20004,7 @@
       </c>
       <c r="T207" s="16"/>
       <c r="U207" s="34" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="208" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20128,7 +20130,7 @@
       </c>
       <c r="T209" s="16"/>
       <c r="U209" s="34" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="210" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20163,7 +20165,7 @@
         <v>12</v>
       </c>
       <c r="K210" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="L210" s="16">
         <v>873</v>
@@ -20191,7 +20193,7 @@
       </c>
       <c r="T210" s="16"/>
       <c r="U210" s="34" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="211" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20502,7 +20504,7 @@
       </c>
       <c r="T215" s="16"/>
       <c r="U215" s="34" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="216" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20626,7 +20628,7 @@
       </c>
       <c r="T217" s="16"/>
       <c r="U217" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="218" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -21920,7 +21922,7 @@
       </c>
       <c r="T238" s="16"/>
       <c r="U238" s="34" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="239" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22107,7 +22109,7 @@
       </c>
       <c r="T241" s="16"/>
       <c r="U241" s="34" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="242" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22431,7 +22433,7 @@
         <v>1</v>
       </c>
       <c r="U246" s="34" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="247" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22744,7 +22746,7 @@
       </c>
       <c r="T251" s="16"/>
       <c r="U251" s="34" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="252" spans="1:21" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -22807,7 +22809,7 @@
       </c>
       <c r="T252" s="42"/>
       <c r="U252" s="43" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -22865,10 +22867,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="56" t="s">
+        <v>779</v>
+      </c>
+      <c r="H1" s="46" t="s">
         <v>780</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>781</v>
       </c>
       <c r="I1" s="46" t="s">
         <v>543</v>
@@ -22883,7 +22885,7 @@
         <v>473</v>
       </c>
       <c r="M1" s="46" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N1" s="46" t="s">
         <v>471</v>
@@ -22898,16 +22900,16 @@
         <v>542</v>
       </c>
       <c r="R1" s="47" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="S1" s="48" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="T1" s="48" t="s">
         <v>624</v>
       </c>
       <c r="U1" s="46" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="V1" s="54"/>
       <c r="W1" s="54"/>
@@ -23974,7 +23976,7 @@
       </c>
       <c r="T18" s="16"/>
       <c r="U18" s="34" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24619,7 +24621,7 @@
         <v>340</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C29" s="16">
         <v>5800</v>
@@ -24644,7 +24646,7 @@
         <v>22</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L29" s="49">
         <v>1567</v>
@@ -24666,14 +24668,14 @@
         <v>1975</v>
       </c>
       <c r="R29" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S29" s="16">
         <v>1</v>
       </c>
       <c r="T29" s="16"/>
       <c r="U29" s="34" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24682,7 +24684,7 @@
         <v>341</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C30" s="16">
         <v>7640</v>
@@ -24707,7 +24709,7 @@
         <v>22</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L30" s="49">
         <v>1576</v>
@@ -24729,14 +24731,14 @@
         <v>1975</v>
       </c>
       <c r="R30" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S30" s="16">
         <v>1</v>
       </c>
       <c r="T30" s="16"/>
       <c r="U30" s="34" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24745,7 +24747,7 @@
         <v>342</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C31" s="16">
         <v>4790</v>
@@ -24770,7 +24772,7 @@
         <v>22</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L31" s="49">
         <v>1566</v>
@@ -24792,14 +24794,14 @@
         <v>1975</v>
       </c>
       <c r="R31" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S31" s="16">
         <v>1</v>
       </c>
       <c r="T31" s="16"/>
       <c r="U31" s="34" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24808,7 +24810,7 @@
         <v>343</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C32" s="16">
         <v>2820</v>
@@ -24833,7 +24835,7 @@
         <v>22</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L32" s="49">
         <v>1535</v>
@@ -24855,14 +24857,14 @@
         <v>1975</v>
       </c>
       <c r="R32" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S32" s="16">
         <v>1</v>
       </c>
       <c r="T32" s="16"/>
       <c r="U32" s="34" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24871,7 +24873,7 @@
         <v>344</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C33" s="16">
         <v>9195</v>
@@ -24896,7 +24898,7 @@
         <v>22</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L33" s="49">
         <v>1491</v>
@@ -24918,14 +24920,14 @@
         <v>1975</v>
       </c>
       <c r="R33" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S33" s="16">
         <v>1</v>
       </c>
       <c r="T33" s="16"/>
       <c r="U33" s="34" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24934,7 +24936,7 @@
         <v>345</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C34" s="16">
         <v>19450</v>
@@ -24959,7 +24961,7 @@
         <v>22</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="L34" s="49">
         <v>1577</v>
@@ -24981,14 +24983,14 @@
         <v>1975</v>
       </c>
       <c r="R34" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S34" s="16">
         <v>1</v>
       </c>
       <c r="T34" s="16"/>
       <c r="U34" s="34" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24997,7 +24999,7 @@
         <v>346</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C35" s="16">
         <v>4300</v>
@@ -25022,7 +25024,7 @@
         <v>22</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L35" s="49">
         <v>1467</v>
@@ -25044,14 +25046,14 @@
         <v>1975</v>
       </c>
       <c r="R35" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S35" s="16">
         <v>1</v>
       </c>
       <c r="T35" s="16"/>
       <c r="U35" s="34" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25060,7 +25062,7 @@
         <v>347</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C36" s="16">
         <v>3030</v>
@@ -25085,7 +25087,7 @@
         <v>22</v>
       </c>
       <c r="K36" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L36" s="49">
         <v>1457</v>
@@ -25107,14 +25109,14 @@
         <v>1975</v>
       </c>
       <c r="R36" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S36" s="16">
         <v>1</v>
       </c>
       <c r="T36" s="16"/>
       <c r="U36" s="34" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25123,7 +25125,7 @@
         <v>348</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C37" s="16">
         <v>6500</v>
@@ -25148,7 +25150,7 @@
         <v>22</v>
       </c>
       <c r="K37" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L37" s="49">
         <v>1589</v>
@@ -25170,14 +25172,14 @@
         <v>1975</v>
       </c>
       <c r="R37" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="S37" s="16">
         <v>1</v>
       </c>
       <c r="T37" s="16"/>
       <c r="U37" s="34" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25186,7 +25188,7 @@
         <v>349</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C38" s="16">
         <v>4200</v>
@@ -25211,7 +25213,7 @@
         <v>22</v>
       </c>
       <c r="K38" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L38" s="49">
         <v>1543</v>
@@ -25240,7 +25242,7 @@
       </c>
       <c r="T38" s="16"/>
       <c r="U38" s="34" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25249,7 +25251,7 @@
         <v>350</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C39" s="16">
         <v>1.5</v>
@@ -25276,7 +25278,7 @@
         <v>22</v>
       </c>
       <c r="K39" s="34" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="L39" s="49">
         <v>640</v>
@@ -25305,7 +25307,7 @@
       </c>
       <c r="T39" s="16"/>
       <c r="U39" s="34" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25314,7 +25316,7 @@
         <v>351</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C40" s="16">
         <v>267</v>
@@ -25342,7 +25344,7 @@
         <v>22</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L40" s="49">
         <v>919</v>
@@ -25371,7 +25373,7 @@
       </c>
       <c r="T40" s="16"/>
       <c r="U40" s="34" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25380,7 +25382,7 @@
         <v>352</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C41" s="16">
         <v>1117</v>
@@ -25393,7 +25395,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="57" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H41" s="16">
         <v>-32</v>
@@ -25403,7 +25405,7 @@
         <v>22</v>
       </c>
       <c r="K41" s="34" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L41" s="49">
         <v>1483</v>
@@ -25432,7 +25434,7 @@
       </c>
       <c r="T41" s="16"/>
       <c r="U41" s="34" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25441,7 +25443,7 @@
         <v>353</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C42" s="16">
         <v>0.19</v>
@@ -25468,7 +25470,7 @@
         <v>22</v>
       </c>
       <c r="K42" s="34" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="L42" s="49">
         <v>1060</v>
@@ -25497,7 +25499,7 @@
       </c>
       <c r="T42" s="16"/>
       <c r="U42" s="34" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25506,7 +25508,7 @@
         <v>354</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C43" s="16">
         <v>0.12</v>
@@ -25533,7 +25535,7 @@
         <v>22</v>
       </c>
       <c r="K43" s="34" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L43" s="49">
         <v>1060</v>
@@ -25562,7 +25564,7 @@
       </c>
       <c r="T43" s="16"/>
       <c r="U43" s="34" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25571,7 +25573,7 @@
         <v>355</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C44" s="16">
         <v>13.3</v>
@@ -25598,7 +25600,7 @@
         <v>22</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="L44" s="49">
         <v>2480</v>
@@ -25629,7 +25631,7 @@
       </c>
       <c r="T44" s="16"/>
       <c r="U44" s="34" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25638,7 +25640,7 @@
         <v>356</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C45" s="16">
         <v>200</v>
@@ -25667,7 +25669,7 @@
         <v>17</v>
       </c>
       <c r="K45" s="34" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="L45" s="49">
         <v>1973</v>
@@ -25696,7 +25698,7 @@
       </c>
       <c r="T45" s="16"/>
       <c r="U45" s="34" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -25705,7 +25707,7 @@
         <v>357</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C46" s="42">
         <v>9.7000000000000003E-2</v>
@@ -25733,7 +25735,7 @@
         <v>12</v>
       </c>
       <c r="K46" s="43" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="L46" s="51">
         <v>1350</v>
@@ -25762,7 +25764,7 @@
       </c>
       <c r="T46" s="42"/>
       <c r="U46" s="43" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further updates on paper, response and data
</commit_message>
<xml_diff>
--- a/data/AllData_Catchments.xlsx
+++ b/data/AllData_Catchments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C082251D-7125-4254-9741-4E6504B50036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57624532-6894-45CE-A0DF-25CC11C05C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2760" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2764" uniqueCount="801">
   <si>
     <t>Watershed #</t>
   </si>
@@ -1872,9 +1872,6 @@
     <t>Van Haveren (1988) does not give coordinates, but one of the original Bates and Hendry (1921)papers does: https://doi.org/10.1175/1520-0493(1921)49&lt;637:SAWWGC&gt;2.0.CO;2</t>
   </si>
   <si>
-    <t>The paper suggests a change in cover of 85% and also a negative value, not a positive. It also is not totally clear how the delta Q is calculated, presumably from Table 4 in the paper. Ths study period is also very short</t>
-  </si>
-  <si>
     <t>159, 160, 165, 239, 240 and 268 are all Yambulla state forest. The location details refer to the overall location not the individual catchments</t>
   </si>
   <si>
@@ -2490,6 +2487,15 @@
   </si>
   <si>
     <t>This is Ruprecht and Schofield (1989) rather than Ruprecht and Schofield (1991). Additionally Delta_Forest changed to -100% as the original paper clearly indicates "clearfelling"</t>
+  </si>
+  <si>
+    <t>The paper suggests a change in cover of 85% and also a negative value, not a positive. It also is not totally clear how the delta Q is calculated, presumably from Table 4 in the paper. Ths study period is also very short. Changed delta F to -85</t>
+  </si>
+  <si>
+    <t>Watson et al. 2001 clearly states that this is clearing followed by reseeding at different densities, changed to -75</t>
+  </si>
+  <si>
+    <t>Ruprecht et al 1989 says "clearfelling", so the change in forestry should be -100 not +100. Bari et al. also says "cleared".</t>
   </si>
 </sst>
 </file>
@@ -3189,10 +3195,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="37" t="s">
+        <v>778</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>779</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>780</v>
       </c>
       <c r="I1" s="37" t="s">
         <v>543</v>
@@ -3207,7 +3213,7 @@
         <v>473</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="N1" s="37" t="s">
         <v>471</v>
@@ -3222,16 +3228,16 @@
         <v>542</v>
       </c>
       <c r="R1" s="38" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="S1" s="38" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="T1" s="37" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="U1" s="39" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
@@ -3294,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="28" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
@@ -6995,7 +7001,7 @@
     </row>
     <row r="63" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
   </sheetData>
@@ -7010,8 +7016,8 @@
   <dimension ref="A1:V252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H153" sqref="H153"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -7051,10 +7057,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="36" t="s">
+        <v>778</v>
+      </c>
+      <c r="H1" s="36" t="s">
         <v>779</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>780</v>
       </c>
       <c r="I1" s="36" t="s">
         <v>543</v>
@@ -7069,7 +7075,7 @@
         <v>473</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="N1" s="36" t="s">
         <v>471</v>
@@ -7084,16 +7090,16 @@
         <v>542</v>
       </c>
       <c r="R1" s="38" t="s">
+        <v>791</v>
+      </c>
+      <c r="S1" s="37" t="s">
+        <v>796</v>
+      </c>
+      <c r="T1" s="37" t="s">
+        <v>623</v>
+      </c>
+      <c r="U1" s="36" t="s">
         <v>792</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>797</v>
-      </c>
-      <c r="T1" s="37" t="s">
-        <v>624</v>
-      </c>
-      <c r="U1" s="36" t="s">
-        <v>793</v>
       </c>
       <c r="V1" s="31"/>
     </row>
@@ -7158,7 +7164,7 @@
       </c>
       <c r="T2" s="16"/>
       <c r="U2" s="34" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="V2" s="32"/>
     </row>
@@ -7223,7 +7229,7 @@
       </c>
       <c r="T3" s="16"/>
       <c r="U3" s="34" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="V3" s="32"/>
     </row>
@@ -7446,7 +7452,7 @@
         <v>12</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="L7" s="49">
         <v>1967</v>
@@ -7474,7 +7480,7 @@
       </c>
       <c r="T7" s="16"/>
       <c r="U7" s="34" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="V7" s="32"/>
     </row>
@@ -7538,7 +7544,7 @@
       </c>
       <c r="T8" s="16"/>
       <c r="U8" s="34" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="V8" s="32"/>
     </row>
@@ -7602,7 +7608,7 @@
       </c>
       <c r="T9" s="16"/>
       <c r="U9" s="34" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -7853,7 +7859,7 @@
       </c>
       <c r="T13" s="16"/>
       <c r="U13" s="34" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -7951,7 +7957,7 @@
         <v>12</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="L15" s="49">
         <v>510</v>
@@ -7979,7 +7985,7 @@
       </c>
       <c r="T15" s="16"/>
       <c r="U15" s="34" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8043,7 +8049,7 @@
       </c>
       <c r="T16" s="16"/>
       <c r="U16" s="34" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8106,7 +8112,7 @@
       </c>
       <c r="T17" s="16"/>
       <c r="U17" s="34" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8169,7 +8175,7 @@
       </c>
       <c r="T18" s="16"/>
       <c r="U18" s="34" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8232,7 +8238,7 @@
       </c>
       <c r="T19" s="16"/>
       <c r="U19" s="34" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8677,7 +8683,7 @@
       </c>
       <c r="T26" s="16"/>
       <c r="U26" s="34" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8740,7 +8746,7 @@
       </c>
       <c r="T27" s="16"/>
       <c r="U27" s="34" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8867,7 +8873,7 @@
       </c>
       <c r="T29" s="16"/>
       <c r="U29" s="34" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -8923,7 +8929,7 @@
         <v>1984</v>
       </c>
       <c r="R30" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S30" s="16">
         <v>1</v>
@@ -9056,7 +9062,7 @@
       </c>
       <c r="T32" s="16"/>
       <c r="U32" s="34" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -9278,7 +9284,7 @@
         <v>12</v>
       </c>
       <c r="K36" s="40" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="L36" s="16">
         <v>1814</v>
@@ -9367,7 +9373,7 @@
       </c>
       <c r="T37" s="16"/>
       <c r="U37" s="34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -9674,7 +9680,7 @@
       </c>
       <c r="T42" s="16"/>
       <c r="U42" s="34" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -9990,7 +9996,7 @@
       </c>
       <c r="T47" s="16"/>
       <c r="U47" s="34" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10025,7 +10031,7 @@
         <v>12</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="L48" s="16">
         <v>1302</v>
@@ -10089,7 +10095,7 @@
         <v>12</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="L49" s="16">
         <v>1302</v>
@@ -10181,7 +10187,7 @@
       </c>
       <c r="T50" s="16"/>
       <c r="U50" s="34" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10302,7 +10308,7 @@
         <v>1964</v>
       </c>
       <c r="R52" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S52" s="16">
         <v>1</v>
@@ -10373,7 +10379,7 @@
       </c>
       <c r="T53" s="16"/>
       <c r="U53" s="34" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="54" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10472,7 +10478,7 @@
         <v>12</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="L55" s="16">
         <v>1263</v>
@@ -10500,7 +10506,7 @@
       </c>
       <c r="T55" s="16"/>
       <c r="U55" s="34" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="56" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10535,7 +10541,7 @@
         <v>12</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="L56" s="16">
         <v>1306</v>
@@ -10563,7 +10569,7 @@
       </c>
       <c r="T56" s="16"/>
       <c r="U56" s="34" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="57" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10786,7 +10792,7 @@
         <v>12</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L60" s="16">
         <v>1736</v>
@@ -10814,7 +10820,7 @@
       </c>
       <c r="T60" s="16"/>
       <c r="U60" s="6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -10849,7 +10855,7 @@
         <v>12</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L61" s="16">
         <v>1736</v>
@@ -10877,7 +10883,7 @@
       </c>
       <c r="T61" s="16"/>
       <c r="U61" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="62" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -11002,7 +11008,7 @@
       </c>
       <c r="T63" s="16"/>
       <c r="U63" s="34" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -11222,7 +11228,7 @@
         <v>12</v>
       </c>
       <c r="K67" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L67" s="16">
         <v>1747</v>
@@ -11250,7 +11256,7 @@
       </c>
       <c r="T67" s="16"/>
       <c r="U67" s="34" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="68" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -11313,7 +11319,7 @@
       </c>
       <c r="T68" s="16"/>
       <c r="U68" s="34" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="69" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -11376,7 +11382,7 @@
       </c>
       <c r="T69" s="16"/>
       <c r="U69" s="34" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="70" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -11439,7 +11445,7 @@
       </c>
       <c r="T70" s="16"/>
       <c r="U70" s="34" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -11565,7 +11571,7 @@
       </c>
       <c r="T72" s="16"/>
       <c r="U72" s="34" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="73" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -11939,7 +11945,7 @@
         <v>149</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C79" s="6">
         <v>0.24</v>
@@ -11966,7 +11972,7 @@
         <v>12</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="L79" s="16">
         <v>1091</v>
@@ -11994,7 +12000,7 @@
       </c>
       <c r="T79" s="16"/>
       <c r="U79" s="34" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="80" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12002,7 +12008,7 @@
         <v>134</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C80" s="6">
         <v>0.15</v>
@@ -12059,7 +12065,7 @@
         <v>1</v>
       </c>
       <c r="U80" s="34" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="81" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12067,7 +12073,7 @@
         <v>137</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C81" s="6">
         <v>0.34</v>
@@ -12131,7 +12137,7 @@
         <v>139</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C82" s="6">
         <v>0.39</v>
@@ -12186,7 +12192,7 @@
       </c>
       <c r="T82" s="16"/>
       <c r="U82" s="34" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="83" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12194,7 +12200,7 @@
         <v>142</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C83" s="6">
         <v>0.22</v>
@@ -12249,7 +12255,7 @@
       </c>
       <c r="T83" s="16"/>
       <c r="U83" s="34" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="84" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12257,7 +12263,7 @@
         <v>143</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C84" s="6">
         <v>0.24</v>
@@ -12318,7 +12324,7 @@
         <v>144</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C85" s="6">
         <v>0.3</v>
@@ -12373,7 +12379,7 @@
       </c>
       <c r="T85" s="16"/>
       <c r="U85" s="34" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="86" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12381,7 +12387,7 @@
         <v>145</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C86" s="6">
         <v>0.15</v>
@@ -12408,7 +12414,7 @@
         <v>12</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="L86" s="16">
         <v>1089</v>
@@ -12438,7 +12444,7 @@
         <v>1</v>
       </c>
       <c r="U86" s="34" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="87" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12446,7 +12452,7 @@
         <v>146</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C87" s="6">
         <v>0.34</v>
@@ -12473,7 +12479,7 @@
         <v>12</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="L87" s="16">
         <v>1089</v>
@@ -12503,7 +12509,7 @@
         <v>1</v>
       </c>
       <c r="U87" s="34" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="88" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12511,7 +12517,7 @@
         <v>147</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C88" s="6">
         <v>0.36</v>
@@ -12538,7 +12544,7 @@
         <v>12</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="L88" s="16">
         <v>1089</v>
@@ -12566,7 +12572,7 @@
       </c>
       <c r="T88" s="16"/>
       <c r="U88" s="34" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="89" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -12574,7 +12580,7 @@
         <v>148</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C89" s="6">
         <v>0.22</v>
@@ -12601,7 +12607,7 @@
         <v>12</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="L89" s="16">
         <v>1089</v>
@@ -12629,7 +12635,7 @@
       </c>
       <c r="T89" s="16"/>
       <c r="U89" s="34" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="90" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -13271,7 +13277,7 @@
         <v>1</v>
       </c>
       <c r="U99" s="34" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="100" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -13336,7 +13342,7 @@
         <v>1</v>
       </c>
       <c r="U100" s="34" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="101" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -13399,7 +13405,7 @@
       </c>
       <c r="T101" s="16"/>
       <c r="U101" s="34" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="102" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -13462,7 +13468,7 @@
       </c>
       <c r="T102" s="16"/>
       <c r="U102" s="34" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="103" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -13525,7 +13531,7 @@
       </c>
       <c r="T103" s="16"/>
       <c r="U103" s="34" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="104" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -13533,7 +13539,7 @@
         <v>164</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C104" s="6">
         <v>0.33</v>
@@ -13589,7 +13595,7 @@
       </c>
       <c r="T104" s="16"/>
       <c r="U104" s="34" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="105" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -13654,7 +13660,7 @@
         <v>1</v>
       </c>
       <c r="U105" s="34" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="106" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -13717,7 +13723,7 @@
       </c>
       <c r="T106" s="16"/>
       <c r="U106" s="34" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="107" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14123,7 +14129,7 @@
         <v>12</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="L113" s="16">
         <v>1217</v>
@@ -14149,7 +14155,7 @@
       </c>
       <c r="T113" s="16"/>
       <c r="U113" s="34" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="114" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14245,7 +14251,7 @@
         <v>12</v>
       </c>
       <c r="K115" s="6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="L115" s="16">
         <v>1217</v>
@@ -14274,7 +14280,7 @@
       </c>
       <c r="T115" s="16"/>
       <c r="U115" s="34" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="V115" s="32"/>
     </row>
@@ -14310,7 +14316,7 @@
         <v>12</v>
       </c>
       <c r="K116" s="6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="L116" s="16">
         <v>1217</v>
@@ -14339,7 +14345,7 @@
       </c>
       <c r="T116" s="16"/>
       <c r="U116" s="34" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="117" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14402,7 +14408,7 @@
       </c>
       <c r="T117" s="16"/>
       <c r="U117" s="34" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="118" spans="1:22" s="13" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14527,7 +14533,7 @@
       </c>
       <c r="T119" s="16"/>
       <c r="U119" s="34" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="120" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14591,7 +14597,7 @@
       </c>
       <c r="T120" s="16"/>
       <c r="U120" s="34" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="121" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14654,7 +14660,7 @@
       </c>
       <c r="T121" s="16"/>
       <c r="U121" s="34" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="122" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -14766,10 +14772,10 @@
         <v>5</v>
       </c>
       <c r="P123" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="Q123" s="16" t="s">
         <v>613</v>
-      </c>
-      <c r="Q123" s="16" t="s">
-        <v>614</v>
       </c>
       <c r="R123" s="33" t="s">
         <v>551</v>
@@ -14892,7 +14898,7 @@
       </c>
       <c r="T125" s="16"/>
       <c r="U125" s="34" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="V125" s="32"/>
     </row>
@@ -15017,7 +15023,7 @@
       </c>
       <c r="T127" s="16"/>
       <c r="U127" s="34" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="128" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15078,7 +15084,7 @@
       </c>
       <c r="T128" s="16"/>
       <c r="U128" s="34" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="129" spans="1:22" s="13" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15137,7 +15143,7 @@
         <v>1</v>
       </c>
       <c r="U129" s="34" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="V129" s="32"/>
     </row>
@@ -15395,7 +15401,7 @@
         <v>194</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C134" s="6">
         <v>0.65</v>
@@ -15451,7 +15457,7 @@
       </c>
       <c r="T134" s="16"/>
       <c r="U134" s="34" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="135" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15514,7 +15520,7 @@
       </c>
       <c r="T135" s="16"/>
       <c r="U135" s="34" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="136" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15577,7 +15583,7 @@
       </c>
       <c r="T136" s="16"/>
       <c r="U136" s="34" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="137" spans="1:22" s="13" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15626,7 +15632,7 @@
       </c>
       <c r="T137" s="16"/>
       <c r="U137" s="34" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="V137" s="32"/>
     </row>
@@ -15744,7 +15750,7 @@
         <v>1990</v>
       </c>
       <c r="R139" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S139" s="16">
         <v>1</v>
@@ -15812,7 +15818,7 @@
       </c>
       <c r="T140" s="16"/>
       <c r="U140" s="34" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="141" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -15995,7 +16001,7 @@
       </c>
       <c r="T143" s="16"/>
       <c r="U143" s="34" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="144" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -16244,7 +16250,7 @@
       </c>
       <c r="T147" s="16"/>
       <c r="U147" s="34" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="148" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -16307,7 +16313,7 @@
       </c>
       <c r="T148" s="16"/>
       <c r="U148" s="34" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="149" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -16370,10 +16376,10 @@
       </c>
       <c r="T149" s="16"/>
       <c r="U149" s="34" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="150" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="150" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="6">
         <v>210</v>
       </c>
@@ -16393,7 +16399,7 @@
         <v>10</v>
       </c>
       <c r="G150" s="6">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="H150" s="6">
         <v>147.6</v>
@@ -16433,7 +16439,9 @@
         <v>1</v>
       </c>
       <c r="T150" s="16"/>
-      <c r="U150" s="34"/>
+      <c r="U150" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="151" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A151" s="6">
@@ -16559,7 +16567,7 @@
       <c r="T152" s="16"/>
       <c r="U152" s="34"/>
     </row>
-    <row r="153" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="6">
         <v>213</v>
       </c>
@@ -16579,7 +16587,7 @@
         <v>10</v>
       </c>
       <c r="G153" s="6">
-        <v>75</v>
+        <v>-75</v>
       </c>
       <c r="H153" s="6">
         <v>43</v>
@@ -16606,7 +16614,7 @@
         <v>12</v>
       </c>
       <c r="P153" s="16">
-        <v>1971</v>
+        <v>1977</v>
       </c>
       <c r="Q153" s="16">
         <v>1996</v>
@@ -16618,9 +16626,11 @@
         <v>1</v>
       </c>
       <c r="T153" s="16"/>
-      <c r="U153" s="34"/>
-    </row>
-    <row r="154" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="U153" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="6">
         <v>214</v>
       </c>
@@ -16640,7 +16650,7 @@
         <v>10</v>
       </c>
       <c r="G154" s="6">
-        <v>75</v>
+        <v>-75</v>
       </c>
       <c r="H154" s="6">
         <v>104</v>
@@ -16667,7 +16677,7 @@
         <v>12</v>
       </c>
       <c r="P154" s="16">
-        <v>1971</v>
+        <v>1977</v>
       </c>
       <c r="Q154" s="16">
         <v>1996</v>
@@ -16679,9 +16689,11 @@
         <v>1</v>
       </c>
       <c r="T154" s="16"/>
-      <c r="U154" s="34"/>
-    </row>
-    <row r="155" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="U154" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="6">
         <v>215</v>
       </c>
@@ -16701,7 +16713,7 @@
         <v>10</v>
       </c>
       <c r="G155" s="6">
-        <v>75</v>
+        <v>-75</v>
       </c>
       <c r="H155" s="6">
         <v>97</v>
@@ -16728,7 +16740,7 @@
         <v>12</v>
       </c>
       <c r="P155" s="16">
-        <v>1971</v>
+        <v>1977</v>
       </c>
       <c r="Q155" s="16">
         <v>1996</v>
@@ -16740,7 +16752,9 @@
         <v>1</v>
       </c>
       <c r="T155" s="16"/>
-      <c r="U155" s="34"/>
+      <c r="U155" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="156" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="6">
@@ -16932,7 +16946,7 @@
         <v>219</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C159" s="6">
         <v>0.30499999999999999</v>
@@ -16988,7 +17002,7 @@
       </c>
       <c r="T159" s="16"/>
       <c r="U159" s="34" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="160" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17023,7 +17037,7 @@
         <v>12</v>
       </c>
       <c r="K160" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="L160" s="16">
         <v>2087</v>
@@ -17053,7 +17067,7 @@
         <v>1</v>
       </c>
       <c r="U160" s="34" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="161" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17088,7 +17102,7 @@
         <v>12</v>
       </c>
       <c r="K161" s="6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="L161" s="16">
         <v>1849</v>
@@ -17116,7 +17130,7 @@
       </c>
       <c r="T161" s="16"/>
       <c r="U161" s="34" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="162" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17151,7 +17165,7 @@
         <v>12</v>
       </c>
       <c r="K162" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="L162" s="16">
         <v>1165</v>
@@ -17214,7 +17228,7 @@
         <v>12</v>
       </c>
       <c r="K163" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="L163" s="16">
         <v>1165</v>
@@ -17342,7 +17356,7 @@
         <v>12</v>
       </c>
       <c r="K165" s="6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="L165" s="16">
         <v>2701</v>
@@ -17368,7 +17382,7 @@
       </c>
       <c r="T165" s="16"/>
       <c r="U165" s="34" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="V165" s="32"/>
     </row>
@@ -17377,7 +17391,7 @@
         <v>225</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C166" s="6">
         <v>0.05</v>
@@ -17404,7 +17418,7 @@
         <v>12</v>
       </c>
       <c r="K166" s="6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="L166" s="16">
         <v>2701</v>
@@ -17432,7 +17446,7 @@
       </c>
       <c r="T166" s="16"/>
       <c r="U166" s="34" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="167" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17533,7 +17547,7 @@
         <v>12</v>
       </c>
       <c r="K168" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="L168" s="16">
         <v>1543</v>
@@ -17643,7 +17657,7 @@
         <v>10</v>
       </c>
       <c r="G170" s="6">
-        <v>90</v>
+        <v>-85</v>
       </c>
       <c r="H170" s="6">
         <v>50</v>
@@ -17681,7 +17695,7 @@
       </c>
       <c r="T170" s="16"/>
       <c r="U170" s="34" t="s">
-        <v>600</v>
+        <v>798</v>
       </c>
     </row>
     <row r="171" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17780,7 +17794,7 @@
         <v>12</v>
       </c>
       <c r="K172" s="6" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="L172" s="16">
         <v>1491</v>
@@ -17808,7 +17822,7 @@
       </c>
       <c r="T172" s="16"/>
       <c r="U172" s="34" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="173" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17843,7 +17857,7 @@
         <v>12</v>
       </c>
       <c r="K173" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="L173" s="16">
         <v>1429</v>
@@ -17865,14 +17879,14 @@
         <v>1983</v>
       </c>
       <c r="R173" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S173" s="16">
         <v>1</v>
       </c>
       <c r="T173" s="16"/>
       <c r="U173" s="34" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="174" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17907,7 +17921,7 @@
         <v>12</v>
       </c>
       <c r="K174" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="L174" s="16">
         <v>1429</v>
@@ -17929,14 +17943,14 @@
         <v>1983</v>
       </c>
       <c r="R174" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S174" s="16">
         <v>1</v>
       </c>
       <c r="T174" s="16"/>
       <c r="U174" s="34" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="175" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -17971,7 +17985,7 @@
         <v>12</v>
       </c>
       <c r="K175" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="L175" s="16">
         <v>1429</v>
@@ -17993,14 +18007,14 @@
         <v>1983</v>
       </c>
       <c r="R175" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S175" s="16">
         <v>1</v>
       </c>
       <c r="T175" s="16"/>
       <c r="U175" s="34" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="176" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -18096,7 +18110,7 @@
         <v>12</v>
       </c>
       <c r="K177" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="L177" s="16">
         <v>1429</v>
@@ -18118,14 +18132,14 @@
         <v>1983</v>
       </c>
       <c r="R177" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S177" s="16">
         <v>1</v>
       </c>
       <c r="T177" s="16"/>
       <c r="U177" s="34" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="178" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -18160,7 +18174,7 @@
         <v>12</v>
       </c>
       <c r="K178" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="L178" s="16">
         <v>1491</v>
@@ -18188,7 +18202,7 @@
       </c>
       <c r="T178" s="16"/>
       <c r="U178" s="34" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="179" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -18253,7 +18267,7 @@
         <v>1</v>
       </c>
       <c r="U179" s="34" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="180" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -18318,7 +18332,7 @@
         <v>1</v>
       </c>
       <c r="U180" s="34" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="181" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -18415,7 +18429,7 @@
         <v>12</v>
       </c>
       <c r="K182" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="L182" s="16">
         <v>1408</v>
@@ -18568,7 +18582,7 @@
       </c>
       <c r="T184" s="16"/>
       <c r="U184" s="34" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="185" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -18755,7 +18769,7 @@
       </c>
       <c r="T187" s="16"/>
       <c r="U187" s="34" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="188" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -18973,7 +18987,7 @@
         <v>12</v>
       </c>
       <c r="K191" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="L191" s="16">
         <v>1974</v>
@@ -19001,7 +19015,7 @@
       </c>
       <c r="T191" s="16"/>
       <c r="U191" s="34" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="192" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19062,7 +19076,7 @@
       </c>
       <c r="T192" s="16"/>
       <c r="U192" s="34" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="193" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19123,7 +19137,7 @@
       </c>
       <c r="T193" s="16"/>
       <c r="U193" s="34" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="194" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19184,7 +19198,7 @@
       </c>
       <c r="T194" s="16"/>
       <c r="U194" s="34" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="195" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19247,7 +19261,7 @@
       </c>
       <c r="T195" s="16"/>
       <c r="U195" s="34" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="196" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19303,7 +19317,7 @@
         <v>1990</v>
       </c>
       <c r="R196" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S196" s="16">
         <v>1</v>
@@ -19366,7 +19380,7 @@
         <v>1990</v>
       </c>
       <c r="R197" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S197" s="16">
         <v>1</v>
@@ -19436,7 +19450,7 @@
       </c>
       <c r="T198" s="16"/>
       <c r="U198" s="34" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="199" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19444,7 +19458,7 @@
         <v>259</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C199" s="6">
         <v>8.08</v>
@@ -19500,7 +19514,7 @@
       </c>
       <c r="T199" s="16"/>
       <c r="U199" s="34" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="200" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19565,7 +19579,7 @@
         <v>0</v>
       </c>
       <c r="U200" s="34" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="201" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -19880,7 +19894,7 @@
         <v>1</v>
       </c>
       <c r="U205" s="34" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="206" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20004,7 +20018,7 @@
       </c>
       <c r="T207" s="16"/>
       <c r="U207" s="34" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="208" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20075,7 +20089,7 @@
         <v>269</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C209" s="6">
         <v>1.8</v>
@@ -20130,7 +20144,7 @@
       </c>
       <c r="T209" s="16"/>
       <c r="U209" s="34" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="210" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20165,7 +20179,7 @@
         <v>12</v>
       </c>
       <c r="K210" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="L210" s="16">
         <v>873</v>
@@ -20193,7 +20207,7 @@
       </c>
       <c r="T210" s="16"/>
       <c r="U210" s="34" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="211" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20256,7 +20270,7 @@
       </c>
       <c r="T211" s="16"/>
       <c r="U211" s="34" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="212" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20319,7 +20333,7 @@
       </c>
       <c r="T212" s="16"/>
       <c r="U212" s="34" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="213" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20504,7 +20518,7 @@
       </c>
       <c r="T215" s="16"/>
       <c r="U215" s="34" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="216" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20628,7 +20642,7 @@
       </c>
       <c r="T217" s="16"/>
       <c r="U217" s="34" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="218" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -20993,7 +21007,7 @@
       </c>
       <c r="T223" s="16"/>
       <c r="U223" s="34" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="224" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -21641,7 +21655,7 @@
         <v>12</v>
       </c>
       <c r="K234" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="L234" s="49">
         <v>1239</v>
@@ -21705,7 +21719,7 @@
         <v>12</v>
       </c>
       <c r="K235" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="L235" s="49">
         <v>2256</v>
@@ -21733,7 +21747,7 @@
       </c>
       <c r="T235" s="16"/>
       <c r="U235" s="34" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="236" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -21922,7 +21936,7 @@
       </c>
       <c r="T238" s="16"/>
       <c r="U238" s="34" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="239" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22081,7 +22095,7 @@
         <v>12</v>
       </c>
       <c r="K241" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="L241" s="49">
         <v>1746</v>
@@ -22109,7 +22123,7 @@
       </c>
       <c r="T241" s="16"/>
       <c r="U241" s="34" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="242" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22210,7 +22224,7 @@
         <v>12</v>
       </c>
       <c r="K243" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="L243" s="49">
         <v>2087</v>
@@ -22340,7 +22354,7 @@
         <v>12</v>
       </c>
       <c r="K245" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="L245" s="49">
         <v>2087</v>
@@ -22433,7 +22447,7 @@
         <v>1</v>
       </c>
       <c r="U246" s="34" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="247" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22496,7 +22510,7 @@
       </c>
       <c r="T247" s="16"/>
       <c r="U247" s="34" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="248" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22559,7 +22573,7 @@
       </c>
       <c r="T248" s="16"/>
       <c r="U248" s="34" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="249" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22622,7 +22636,7 @@
       </c>
       <c r="T249" s="16"/>
       <c r="U249" s="34" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="250" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22685,7 +22699,7 @@
       </c>
       <c r="T250" s="16"/>
       <c r="U250" s="34" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="251" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -22746,7 +22760,7 @@
       </c>
       <c r="T251" s="16"/>
       <c r="U251" s="34" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="252" spans="1:21" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -22754,7 +22768,7 @@
         <v>312</v>
       </c>
       <c r="B252" s="8" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C252" s="8">
         <v>2.7</v>
@@ -22809,7 +22823,7 @@
       </c>
       <c r="T252" s="42"/>
       <c r="U252" s="43" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
   </sheetData>
@@ -22867,10 +22881,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="56" t="s">
+        <v>778</v>
+      </c>
+      <c r="H1" s="46" t="s">
         <v>779</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>780</v>
       </c>
       <c r="I1" s="46" t="s">
         <v>543</v>
@@ -22885,7 +22899,7 @@
         <v>473</v>
       </c>
       <c r="M1" s="46" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="N1" s="46" t="s">
         <v>471</v>
@@ -22900,16 +22914,16 @@
         <v>542</v>
       </c>
       <c r="R1" s="47" t="s">
+        <v>791</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>796</v>
+      </c>
+      <c r="T1" s="48" t="s">
+        <v>623</v>
+      </c>
+      <c r="U1" s="46" t="s">
         <v>792</v>
-      </c>
-      <c r="S1" s="48" t="s">
-        <v>797</v>
-      </c>
-      <c r="T1" s="48" t="s">
-        <v>624</v>
-      </c>
-      <c r="U1" s="46" t="s">
-        <v>793</v>
       </c>
       <c r="V1" s="54"/>
       <c r="W1" s="54"/>
@@ -23976,7 +23990,7 @@
       </c>
       <c r="T18" s="16"/>
       <c r="U18" s="34" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24612,7 +24626,7 @@
       </c>
       <c r="T28" s="16"/>
       <c r="U28" s="34" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24621,7 +24635,7 @@
         <v>340</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C29" s="16">
         <v>5800</v>
@@ -24646,7 +24660,7 @@
         <v>22</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L29" s="49">
         <v>1567</v>
@@ -24668,14 +24682,14 @@
         <v>1975</v>
       </c>
       <c r="R29" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S29" s="16">
         <v>1</v>
       </c>
       <c r="T29" s="16"/>
       <c r="U29" s="34" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24684,7 +24698,7 @@
         <v>341</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C30" s="16">
         <v>7640</v>
@@ -24709,7 +24723,7 @@
         <v>22</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L30" s="49">
         <v>1576</v>
@@ -24731,14 +24745,14 @@
         <v>1975</v>
       </c>
       <c r="R30" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S30" s="16">
         <v>1</v>
       </c>
       <c r="T30" s="16"/>
       <c r="U30" s="34" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24747,7 +24761,7 @@
         <v>342</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C31" s="16">
         <v>4790</v>
@@ -24772,7 +24786,7 @@
         <v>22</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L31" s="49">
         <v>1566</v>
@@ -24794,14 +24808,14 @@
         <v>1975</v>
       </c>
       <c r="R31" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S31" s="16">
         <v>1</v>
       </c>
       <c r="T31" s="16"/>
       <c r="U31" s="34" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24810,7 +24824,7 @@
         <v>343</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C32" s="16">
         <v>2820</v>
@@ -24835,7 +24849,7 @@
         <v>22</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L32" s="49">
         <v>1535</v>
@@ -24857,14 +24871,14 @@
         <v>1975</v>
       </c>
       <c r="R32" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S32" s="16">
         <v>1</v>
       </c>
       <c r="T32" s="16"/>
       <c r="U32" s="34" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24873,7 +24887,7 @@
         <v>344</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C33" s="16">
         <v>9195</v>
@@ -24898,7 +24912,7 @@
         <v>22</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L33" s="49">
         <v>1491</v>
@@ -24920,14 +24934,14 @@
         <v>1975</v>
       </c>
       <c r="R33" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S33" s="16">
         <v>1</v>
       </c>
       <c r="T33" s="16"/>
       <c r="U33" s="34" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24936,7 +24950,7 @@
         <v>345</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C34" s="16">
         <v>19450</v>
@@ -24961,7 +24975,7 @@
         <v>22</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="L34" s="49">
         <v>1577</v>
@@ -24983,14 +24997,14 @@
         <v>1975</v>
       </c>
       <c r="R34" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S34" s="16">
         <v>1</v>
       </c>
       <c r="T34" s="16"/>
       <c r="U34" s="34" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -24999,7 +25013,7 @@
         <v>346</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C35" s="16">
         <v>4300</v>
@@ -25024,7 +25038,7 @@
         <v>22</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L35" s="49">
         <v>1467</v>
@@ -25046,14 +25060,14 @@
         <v>1975</v>
       </c>
       <c r="R35" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S35" s="16">
         <v>1</v>
       </c>
       <c r="T35" s="16"/>
       <c r="U35" s="34" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25062,7 +25076,7 @@
         <v>347</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C36" s="16">
         <v>3030</v>
@@ -25087,7 +25101,7 @@
         <v>22</v>
       </c>
       <c r="K36" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L36" s="49">
         <v>1457</v>
@@ -25109,14 +25123,14 @@
         <v>1975</v>
       </c>
       <c r="R36" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S36" s="16">
         <v>1</v>
       </c>
       <c r="T36" s="16"/>
       <c r="U36" s="34" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25125,7 +25139,7 @@
         <v>348</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C37" s="16">
         <v>6500</v>
@@ -25150,7 +25164,7 @@
         <v>22</v>
       </c>
       <c r="K37" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L37" s="49">
         <v>1589</v>
@@ -25172,14 +25186,14 @@
         <v>1975</v>
       </c>
       <c r="R37" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="S37" s="16">
         <v>1</v>
       </c>
       <c r="T37" s="16"/>
       <c r="U37" s="34" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25188,7 +25202,7 @@
         <v>349</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C38" s="16">
         <v>4200</v>
@@ -25213,7 +25227,7 @@
         <v>22</v>
       </c>
       <c r="K38" s="34" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L38" s="49">
         <v>1543</v>
@@ -25242,7 +25256,7 @@
       </c>
       <c r="T38" s="16"/>
       <c r="U38" s="34" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25251,7 +25265,7 @@
         <v>350</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C39" s="16">
         <v>1.5</v>
@@ -25278,7 +25292,7 @@
         <v>22</v>
       </c>
       <c r="K39" s="34" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="L39" s="49">
         <v>640</v>
@@ -25307,7 +25321,7 @@
       </c>
       <c r="T39" s="16"/>
       <c r="U39" s="34" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25316,7 +25330,7 @@
         <v>351</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C40" s="16">
         <v>267</v>
@@ -25344,7 +25358,7 @@
         <v>22</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="L40" s="49">
         <v>919</v>
@@ -25373,7 +25387,7 @@
       </c>
       <c r="T40" s="16"/>
       <c r="U40" s="34" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25382,7 +25396,7 @@
         <v>352</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C41" s="16">
         <v>1117</v>
@@ -25395,7 +25409,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="57" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="H41" s="16">
         <v>-32</v>
@@ -25405,7 +25419,7 @@
         <v>22</v>
       </c>
       <c r="K41" s="34" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L41" s="49">
         <v>1483</v>
@@ -25434,7 +25448,7 @@
       </c>
       <c r="T41" s="16"/>
       <c r="U41" s="34" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25443,7 +25457,7 @@
         <v>353</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C42" s="16">
         <v>0.19</v>
@@ -25470,7 +25484,7 @@
         <v>22</v>
       </c>
       <c r="K42" s="34" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="L42" s="49">
         <v>1060</v>
@@ -25499,7 +25513,7 @@
       </c>
       <c r="T42" s="16"/>
       <c r="U42" s="34" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25508,7 +25522,7 @@
         <v>354</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C43" s="16">
         <v>0.12</v>
@@ -25535,7 +25549,7 @@
         <v>22</v>
       </c>
       <c r="K43" s="34" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L43" s="49">
         <v>1060</v>
@@ -25564,7 +25578,7 @@
       </c>
       <c r="T43" s="16"/>
       <c r="U43" s="34" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25573,7 +25587,7 @@
         <v>355</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C44" s="16">
         <v>13.3</v>
@@ -25600,7 +25614,7 @@
         <v>22</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L44" s="49">
         <v>2480</v>
@@ -25631,7 +25645,7 @@
       </c>
       <c r="T44" s="16"/>
       <c r="U44" s="34" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -25640,7 +25654,7 @@
         <v>356</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C45" s="16">
         <v>200</v>
@@ -25669,7 +25683,7 @@
         <v>17</v>
       </c>
       <c r="K45" s="34" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="L45" s="49">
         <v>1973</v>
@@ -25698,7 +25712,7 @@
       </c>
       <c r="T45" s="16"/>
       <c r="U45" s="34" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -25707,7 +25721,7 @@
         <v>357</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C46" s="42">
         <v>9.7000000000000003E-2</v>
@@ -25735,7 +25749,7 @@
         <v>12</v>
       </c>
       <c r="K46" s="43" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L46" s="51">
         <v>1350</v>
@@ -25764,7 +25778,7 @@
       </c>
       <c r="T46" s="42"/>
       <c r="U46" s="43" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress in updating the paper 09082022
</commit_message>
<xml_diff>
--- a/data/AllData_Catchments.xlsx
+++ b/data/AllData_Catchments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82491655-3B3C-4BCD-8238-766AF99DCF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4EF6C8C-7562-471F-92E7-B9247E37EB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LargeCatchments_T1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LargeCatchments_T1!$L$1:$L$63</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewCatchments_T3!$L$1:$L$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SmallCatchments_T2!$L$1:$L$252</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SmallCatchments_T2!$H$1:$H$252</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,6 +34,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="820">
   <si>
     <t>Watershed #</t>
   </si>
@@ -2522,11 +2523,38 @@
   <si>
     <t>Correct name is Yerraminnup S..There is no Yerrami S in Zhou et al. This is originally from Ruprecht and Schofield (1989), but they are citing a WA water resources report, Dates confirmed in the original. Also, this is clearing, so should be -60% delta_F_perc</t>
   </si>
+  <si>
+    <t>Ferreto et al., 2021</t>
+  </si>
+  <si>
+    <t>PE30 = Old-EsW</t>
+  </si>
+  <si>
+    <t>PE100 = Young-EbW</t>
+  </si>
+  <si>
+    <t>Almeida et al., 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitored from 34 month before harvest, to 14 month after harvest. Pa &amp; DQf calculated fron discharge in Table II (mm) (433-483)/483=-10%. E0 from Table III. </t>
+  </si>
+  <si>
+    <t>Monitored 4 years after harvest and replanting. Also correcting Almeida´s %for is 30% of the 61% of eucalyptus area. Pa &amp; E0 from Table 2</t>
+  </si>
+  <si>
+    <t>Monitored 4 years after harvest and replanting. Also correcting Almeida´s %for is 100% of the 65% of eucalyptus area. Pa &amp; E0 from Table 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitored from 34 month before harvest, to 14 month after harvest. Pa &amp; DQf calculated fron discharge in Table II (mm) (459/424-248/1027)/(248/1027)=+85%. E0 from Table III. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2685,7 +2713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -2851,6 +2879,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3164,15 +3195,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CA6CB8-28F4-480A-8011-F310B3E1710B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="12" width="15.59765625" style="2"/>
     <col min="13" max="14" width="15.59765625" style="4"/>
@@ -3182,7 +3213,7 @@
     <col min="23" max="16384" width="15.59765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="8" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="8" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -3247,7 +3278,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3310,7 +3341,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3373,7 +3404,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3436,7 +3467,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3499,7 +3530,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3562,7 +3593,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3623,7 +3654,7 @@
       </c>
       <c r="U7" s="27"/>
     </row>
-    <row r="8" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3684,7 +3715,7 @@
       </c>
       <c r="U8" s="27"/>
     </row>
-    <row r="9" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3745,7 +3776,7 @@
       </c>
       <c r="U9" s="27"/>
     </row>
-    <row r="10" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3808,7 +3839,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3869,7 +3900,7 @@
       </c>
       <c r="U11" s="27"/>
     </row>
-    <row r="12" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3930,7 +3961,7 @@
       </c>
       <c r="U12" s="27"/>
     </row>
-    <row r="13" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3991,7 +4022,7 @@
       </c>
       <c r="U13" s="27"/>
     </row>
-    <row r="14" spans="1:21" s="5" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="5" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>13</v>
       </c>
@@ -4054,7 +4085,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4115,7 +4146,7 @@
       </c>
       <c r="U15" s="27"/>
     </row>
-    <row r="16" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4178,7 +4209,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4240,7 +4271,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4303,7 +4334,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4364,7 +4395,7 @@
       </c>
       <c r="U19" s="27"/>
     </row>
-    <row r="20" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4425,7 +4456,7 @@
       </c>
       <c r="U20" s="27"/>
     </row>
-    <row r="21" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4486,7 +4517,7 @@
       </c>
       <c r="U21" s="27"/>
     </row>
-    <row r="22" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4549,7 +4580,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4612,7 +4643,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4675,7 +4706,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4737,7 +4768,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4800,7 +4831,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4859,7 +4890,7 @@
       </c>
       <c r="U27" s="27"/>
     </row>
-    <row r="28" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4922,7 +4953,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4981,7 +5012,7 @@
       </c>
       <c r="U29" s="27"/>
     </row>
-    <row r="30" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5042,7 +5073,7 @@
       </c>
       <c r="U30" s="27"/>
     </row>
-    <row r="31" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5103,7 +5134,7 @@
       </c>
       <c r="U31" s="27"/>
     </row>
-    <row r="32" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5164,7 +5195,7 @@
       </c>
       <c r="U32" s="27"/>
     </row>
-    <row r="33" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5227,7 +5258,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5288,7 +5319,7 @@
       </c>
       <c r="U34" s="27"/>
     </row>
-    <row r="35" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5347,7 +5378,7 @@
       </c>
       <c r="U35" s="27"/>
     </row>
-    <row r="36" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5406,7 +5437,7 @@
       </c>
       <c r="U36" s="27"/>
     </row>
-    <row r="37" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5467,7 +5498,7 @@
       </c>
       <c r="U37" s="27"/>
     </row>
-    <row r="38" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5527,7 +5558,7 @@
       </c>
       <c r="U38" s="27"/>
     </row>
-    <row r="39" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5588,7 +5619,7 @@
       </c>
       <c r="U39" s="27"/>
     </row>
-    <row r="40" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -5649,7 +5680,7 @@
       </c>
       <c r="U40" s="27"/>
     </row>
-    <row r="41" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -5710,7 +5741,7 @@
       </c>
       <c r="U41" s="27"/>
     </row>
-    <row r="42" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -5773,7 +5804,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -5836,7 +5867,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -5898,7 +5929,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -5960,7 +5991,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -6020,7 +6051,7 @@
       </c>
       <c r="U46" s="27"/>
     </row>
-    <row r="47" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -6083,7 +6114,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -6145,7 +6176,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -6208,7 +6239,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -6269,7 +6300,7 @@
       </c>
       <c r="U50" s="27"/>
     </row>
-    <row r="51" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -6332,7 +6363,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -6395,7 +6426,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -6456,7 +6487,7 @@
       </c>
       <c r="U53" s="27"/>
     </row>
-    <row r="54" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -6515,7 +6546,7 @@
       </c>
       <c r="U54" s="27"/>
     </row>
-    <row r="55" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -6578,7 +6609,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -6639,7 +6670,7 @@
       </c>
       <c r="U56" s="27"/>
     </row>
-    <row r="57" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -6700,7 +6731,7 @@
       </c>
       <c r="U57" s="27"/>
     </row>
-    <row r="58" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -6759,7 +6790,7 @@
       </c>
       <c r="U58" s="27"/>
     </row>
-    <row r="59" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -6820,7 +6851,7 @@
       </c>
       <c r="U59" s="27"/>
     </row>
-    <row r="60" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -6880,7 +6911,7 @@
       </c>
       <c r="U60" s="27"/>
     </row>
-    <row r="61" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -6943,7 +6974,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="21">
         <v>61</v>
       </c>
@@ -7006,33 +7037,31 @@
         <v>529</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>761</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="L1:L63" xr:uid="{29CA6CB8-28F4-480A-8011-F310B3E1710B}"/>
+  <autoFilter ref="L1:L63" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AFE286-8638-404F-9DBC-2F4BDB10044C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V252"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A129" sqref="A1:U252"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.59765625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.53125" style="2" customWidth="1"/>
-    <col min="3" max="10" width="15.59765625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.53125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="15.59765625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.59765625" style="15" customWidth="1"/>
     <col min="13" max="14" width="15.59765625" style="9" customWidth="1"/>
     <col min="15" max="17" width="15.59765625" style="2" customWidth="1"/>
@@ -7044,7 +7073,7 @@
     <col min="23" max="16384" width="10.59765625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="39" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" s="39" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7110,7 +7139,7 @@
       </c>
       <c r="V1" s="30"/>
     </row>
-    <row r="2" spans="1:22" s="40" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>62</v>
       </c>
@@ -7174,7 +7203,7 @@
       </c>
       <c r="V2" s="31"/>
     </row>
-    <row r="3" spans="1:22" s="40" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>63</v>
       </c>
@@ -7238,7 +7267,7 @@
       </c>
       <c r="V3" s="31"/>
     </row>
-    <row r="4" spans="1:22" s="40" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>64</v>
       </c>
@@ -7300,7 +7329,7 @@
       <c r="U4"/>
       <c r="V4" s="31"/>
     </row>
-    <row r="5" spans="1:22" s="40" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>65</v>
       </c>
@@ -7362,7 +7391,7 @@
       <c r="U5"/>
       <c r="V5" s="31"/>
     </row>
-    <row r="6" spans="1:22" s="40" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>66</v>
       </c>
@@ -7424,7 +7453,7 @@
       <c r="U6"/>
       <c r="V6" s="31"/>
     </row>
-    <row r="7" spans="1:22" s="40" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>67</v>
       </c>
@@ -7488,7 +7517,7 @@
       </c>
       <c r="V7" s="31"/>
     </row>
-    <row r="8" spans="1:22" s="40" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>68</v>
       </c>
@@ -7552,7 +7581,7 @@
       </c>
       <c r="V8" s="31"/>
     </row>
-    <row r="9" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>69</v>
       </c>
@@ -7615,7 +7644,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>70</v>
       </c>
@@ -7678,7 +7707,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>71</v>
       </c>
@@ -7741,7 +7770,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>72</v>
       </c>
@@ -7804,7 +7833,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="66">
         <v>73</v>
       </c>
@@ -7867,7 +7896,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>74</v>
       </c>
@@ -7930,7 +7959,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>75</v>
       </c>
@@ -7993,7 +8022,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>76</v>
       </c>
@@ -8056,7 +8085,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>77</v>
       </c>
@@ -8119,7 +8148,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>78</v>
       </c>
@@ -8182,7 +8211,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>79</v>
       </c>
@@ -8245,7 +8274,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>80</v>
       </c>
@@ -8308,7 +8337,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>81</v>
       </c>
@@ -8371,7 +8400,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>82</v>
       </c>
@@ -8434,7 +8463,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>83</v>
       </c>
@@ -8497,7 +8526,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>84</v>
       </c>
@@ -8558,7 +8587,7 @@
       <c r="T24"/>
       <c r="U24"/>
     </row>
-    <row r="25" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>85</v>
       </c>
@@ -8623,7 +8652,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>86</v>
       </c>
@@ -8686,7 +8715,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>87</v>
       </c>
@@ -8749,7 +8778,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>88</v>
       </c>
@@ -8812,7 +8841,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="66">
         <v>89</v>
       </c>
@@ -8875,7 +8904,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>90</v>
       </c>
@@ -8938,7 +8967,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>91</v>
       </c>
@@ -8999,7 +9028,7 @@
       <c r="T31"/>
       <c r="U31"/>
     </row>
-    <row r="32" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>92</v>
       </c>
@@ -9062,7 +9091,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>93</v>
       </c>
@@ -9127,7 +9156,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>94</v>
       </c>
@@ -9190,7 +9219,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>95</v>
       </c>
@@ -9253,7 +9282,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>96</v>
       </c>
@@ -9314,7 +9343,7 @@
       <c r="T36"/>
       <c r="U36"/>
     </row>
-    <row r="37" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="66">
         <v>97</v>
       </c>
@@ -9377,7 +9406,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>98</v>
       </c>
@@ -9438,7 +9467,7 @@
       <c r="T38"/>
       <c r="U38"/>
     </row>
-    <row r="39" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>99</v>
       </c>
@@ -9499,7 +9528,7 @@
       <c r="T39"/>
       <c r="U39"/>
     </row>
-    <row r="40" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>100</v>
       </c>
@@ -9562,7 +9591,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>101</v>
       </c>
@@ -9623,7 +9652,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>102</v>
       </c>
@@ -9686,7 +9715,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>103</v>
       </c>
@@ -9749,7 +9778,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>104</v>
       </c>
@@ -9812,7 +9841,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>105</v>
       </c>
@@ -9875,7 +9904,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>106</v>
       </c>
@@ -9938,7 +9967,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>107</v>
       </c>
@@ -10001,7 +10030,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>108</v>
       </c>
@@ -10064,7 +10093,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>109</v>
       </c>
@@ -10127,7 +10156,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>110</v>
       </c>
@@ -10190,7 +10219,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>111</v>
       </c>
@@ -10253,7 +10282,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>112</v>
       </c>
@@ -10316,7 +10345,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>113</v>
       </c>
@@ -10379,7 +10408,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>114</v>
       </c>
@@ -10442,7 +10471,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>115</v>
       </c>
@@ -10505,7 +10534,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>116</v>
       </c>
@@ -10568,7 +10597,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>117</v>
       </c>
@@ -10631,7 +10660,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>118</v>
       </c>
@@ -10694,7 +10723,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>119</v>
       </c>
@@ -10755,7 +10784,7 @@
       <c r="T59"/>
       <c r="U59"/>
     </row>
-    <row r="60" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>120</v>
       </c>
@@ -10818,7 +10847,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>121</v>
       </c>
@@ -10881,7 +10910,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>122</v>
       </c>
@@ -10942,7 +10971,7 @@
       <c r="T62"/>
       <c r="U62"/>
     </row>
-    <row r="63" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="66">
         <v>123</v>
       </c>
@@ -11005,7 +11034,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>124</v>
       </c>
@@ -11068,7 +11097,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>125</v>
       </c>
@@ -11129,7 +11158,7 @@
       <c r="T65"/>
       <c r="U65"/>
     </row>
-    <row r="66" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>126</v>
       </c>
@@ -11190,7 +11219,7 @@
       <c r="T66"/>
       <c r="U66"/>
     </row>
-    <row r="67" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>127</v>
       </c>
@@ -11253,7 +11282,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>128</v>
       </c>
@@ -11316,7 +11345,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>129</v>
       </c>
@@ -11379,7 +11408,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>130</v>
       </c>
@@ -11442,7 +11471,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>131</v>
       </c>
@@ -11505,7 +11534,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="66">
         <v>132</v>
       </c>
@@ -11568,7 +11597,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>133</v>
       </c>
@@ -11629,7 +11658,7 @@
       <c r="T73"/>
       <c r="U73"/>
     </row>
-    <row r="74" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>134</v>
       </c>
@@ -11694,7 +11723,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>135</v>
       </c>
@@ -11755,7 +11784,7 @@
       <c r="T75"/>
       <c r="U75"/>
     </row>
-    <row r="76" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>136</v>
       </c>
@@ -11816,7 +11845,7 @@
       <c r="T76"/>
       <c r="U76"/>
     </row>
-    <row r="77" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>137</v>
       </c>
@@ -11879,7 +11908,7 @@
       </c>
       <c r="U77"/>
     </row>
-    <row r="78" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>138</v>
       </c>
@@ -11940,7 +11969,7 @@
       <c r="T78"/>
       <c r="U78"/>
     </row>
-    <row r="79" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>139</v>
       </c>
@@ -12003,7 +12032,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>140</v>
       </c>
@@ -12064,7 +12093,7 @@
       <c r="T80"/>
       <c r="U80"/>
     </row>
-    <row r="81" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>141</v>
       </c>
@@ -12125,7 +12154,7 @@
       <c r="T81"/>
       <c r="U81"/>
     </row>
-    <row r="82" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>142</v>
       </c>
@@ -12188,7 +12217,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>143</v>
       </c>
@@ -12249,7 +12278,7 @@
       <c r="T83"/>
       <c r="U83"/>
     </row>
-    <row r="84" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>144</v>
       </c>
@@ -12312,7 +12341,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>145</v>
       </c>
@@ -12377,7 +12406,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>146</v>
       </c>
@@ -12442,7 +12471,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>147</v>
       </c>
@@ -12505,7 +12534,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>148</v>
       </c>
@@ -12568,7 +12597,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>149</v>
       </c>
@@ -12631,7 +12660,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>150</v>
       </c>
@@ -12694,7 +12723,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>151</v>
       </c>
@@ -12759,7 +12788,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>152</v>
       </c>
@@ -12824,7 +12853,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>153</v>
       </c>
@@ -12889,7 +12918,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>154</v>
       </c>
@@ -12952,7 +12981,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>155</v>
       </c>
@@ -13015,7 +13044,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>156</v>
       </c>
@@ -13080,7 +13109,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>157</v>
       </c>
@@ -13145,7 +13174,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="98" spans="1:22" s="12" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>158</v>
       </c>
@@ -13203,7 +13232,7 @@
       </c>
       <c r="V98" s="31"/>
     </row>
-    <row r="99" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>159</v>
       </c>
@@ -13268,7 +13297,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="100" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>160</v>
       </c>
@@ -13333,7 +13362,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="66">
         <v>161</v>
       </c>
@@ -13396,7 +13425,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="66">
         <v>162</v>
       </c>
@@ -13459,7 +13488,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="103" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="66">
         <v>163</v>
       </c>
@@ -13522,7 +13551,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>164</v>
       </c>
@@ -13585,7 +13614,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="105" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>165</v>
       </c>
@@ -13650,7 +13679,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="106" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>166</v>
       </c>
@@ -13713,7 +13742,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>167</v>
       </c>
@@ -13774,7 +13803,7 @@
       <c r="T107"/>
       <c r="U107"/>
     </row>
-    <row r="108" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>168</v>
       </c>
@@ -13837,7 +13866,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="109" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>169</v>
       </c>
@@ -13898,7 +13927,7 @@
       <c r="T109"/>
       <c r="U109"/>
     </row>
-    <row r="110" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>170</v>
       </c>
@@ -13961,7 +13990,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="111" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>171</v>
       </c>
@@ -14022,7 +14051,7 @@
       <c r="T111"/>
       <c r="U111"/>
     </row>
-    <row r="112" spans="1:22" s="12" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>172</v>
       </c>
@@ -14084,7 +14113,7 @@
       <c r="U112"/>
       <c r="V112" s="31"/>
     </row>
-    <row r="113" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>173</v>
       </c>
@@ -14145,7 +14174,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="114" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>174</v>
       </c>
@@ -14206,7 +14235,7 @@
       <c r="T114"/>
       <c r="U114"/>
     </row>
-    <row r="115" spans="1:22" s="12" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>175</v>
       </c>
@@ -14270,7 +14299,7 @@
       </c>
       <c r="V115" s="31"/>
     </row>
-    <row r="116" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>176</v>
       </c>
@@ -14333,7 +14362,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="117" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>177</v>
       </c>
@@ -14396,7 +14425,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="118" spans="1:22" s="12" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>178</v>
       </c>
@@ -14458,7 +14487,7 @@
       <c r="U118"/>
       <c r="V118" s="31"/>
     </row>
-    <row r="119" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>179</v>
       </c>
@@ -14521,7 +14550,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="120" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>180</v>
       </c>
@@ -14584,7 +14613,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="121" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A121" s="66">
         <v>181</v>
       </c>
@@ -14647,7 +14676,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="122" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>182</v>
       </c>
@@ -14708,7 +14737,7 @@
       <c r="T122"/>
       <c r="U122"/>
     </row>
-    <row r="123" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>183</v>
       </c>
@@ -14769,7 +14798,7 @@
       <c r="T123"/>
       <c r="U123"/>
     </row>
-    <row r="124" spans="1:22" s="13" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:22" s="13" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>184</v>
       </c>
@@ -14835,7 +14864,7 @@
       </c>
       <c r="V124" s="31"/>
     </row>
-    <row r="125" spans="1:22" s="12" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>185</v>
       </c>
@@ -14885,7 +14914,7 @@
       </c>
       <c r="V125" s="31"/>
     </row>
-    <row r="126" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>186</v>
       </c>
@@ -14946,7 +14975,7 @@
       <c r="T126"/>
       <c r="U126"/>
     </row>
-    <row r="127" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>187</v>
       </c>
@@ -15009,7 +15038,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="128" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A128" s="68">
         <v>188</v>
       </c>
@@ -15070,7 +15099,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="129" spans="1:22" s="12" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>189</v>
       </c>
@@ -15130,7 +15159,7 @@
       </c>
       <c r="V129" s="31"/>
     </row>
-    <row r="130" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>190</v>
       </c>
@@ -15191,7 +15220,7 @@
       <c r="T130"/>
       <c r="U130"/>
     </row>
-    <row r="131" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>191</v>
       </c>
@@ -15254,7 +15283,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="132" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>192</v>
       </c>
@@ -15317,7 +15346,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="133" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>193</v>
       </c>
@@ -15378,7 +15407,7 @@
       <c r="T133"/>
       <c r="U133"/>
     </row>
-    <row r="134" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>194</v>
       </c>
@@ -15441,7 +15470,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="135" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>195</v>
       </c>
@@ -15504,7 +15533,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="136" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>196</v>
       </c>
@@ -15567,7 +15596,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="137" spans="1:22" s="12" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>197</v>
       </c>
@@ -15617,7 +15646,7 @@
       </c>
       <c r="V137" s="31"/>
     </row>
-    <row r="138" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>198</v>
       </c>
@@ -15678,7 +15707,7 @@
       <c r="T138"/>
       <c r="U138"/>
     </row>
-    <row r="139" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>199</v>
       </c>
@@ -15741,7 +15770,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="140" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>200</v>
       </c>
@@ -15802,7 +15831,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="141" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>201</v>
       </c>
@@ -15861,7 +15890,7 @@
       <c r="T141"/>
       <c r="U141"/>
     </row>
-    <row r="142" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>202</v>
       </c>
@@ -15922,7 +15951,7 @@
       <c r="T142"/>
       <c r="U142"/>
     </row>
-    <row r="143" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>203</v>
       </c>
@@ -15985,7 +16014,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="144" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>204</v>
       </c>
@@ -16048,7 +16077,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>205</v>
       </c>
@@ -16109,7 +16138,7 @@
       <c r="T145"/>
       <c r="U145"/>
     </row>
-    <row r="146" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>206</v>
       </c>
@@ -16170,7 +16199,7 @@
       <c r="T146"/>
       <c r="U146"/>
     </row>
-    <row r="147" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>207</v>
       </c>
@@ -16233,7 +16262,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>208</v>
       </c>
@@ -16296,7 +16325,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>209</v>
       </c>
@@ -16359,7 +16388,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>210</v>
       </c>
@@ -16422,7 +16451,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>211</v>
       </c>
@@ -16483,7 +16512,7 @@
       <c r="T151"/>
       <c r="U151"/>
     </row>
-    <row r="152" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>212</v>
       </c>
@@ -16544,7 +16573,7 @@
       <c r="T152"/>
       <c r="U152"/>
     </row>
-    <row r="153" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>213</v>
       </c>
@@ -16607,7 +16636,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>214</v>
       </c>
@@ -16670,7 +16699,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>215</v>
       </c>
@@ -16733,7 +16762,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>216</v>
       </c>
@@ -16794,7 +16823,7 @@
       <c r="T156"/>
       <c r="U156"/>
     </row>
-    <row r="157" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>217</v>
       </c>
@@ -16855,7 +16884,7 @@
       <c r="T157"/>
       <c r="U157"/>
     </row>
-    <row r="158" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>218</v>
       </c>
@@ -16916,7 +16945,7 @@
       <c r="T158"/>
       <c r="U158"/>
     </row>
-    <row r="159" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>219</v>
       </c>
@@ -16979,7 +17008,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>220</v>
       </c>
@@ -17044,7 +17073,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>221</v>
       </c>
@@ -17107,7 +17136,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="162" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>222</v>
       </c>
@@ -17170,7 +17199,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="163" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>223</v>
       </c>
@@ -17235,7 +17264,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="164" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>224</v>
       </c>
@@ -17298,7 +17327,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="165" spans="1:22" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:22" s="11" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>225</v>
       </c>
@@ -17362,7 +17391,7 @@
       </c>
       <c r="V165" s="31"/>
     </row>
-    <row r="166" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>226</v>
       </c>
@@ -17423,7 +17452,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="167" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>227</v>
       </c>
@@ -17488,7 +17517,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>228</v>
       </c>
@@ -17549,7 +17578,7 @@
       <c r="T168"/>
       <c r="U168"/>
     </row>
-    <row r="169" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>229</v>
       </c>
@@ -17610,7 +17639,7 @@
       <c r="T169"/>
       <c r="U169"/>
     </row>
-    <row r="170" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>230</v>
       </c>
@@ -17671,7 +17700,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>231</v>
       </c>
@@ -17734,7 +17763,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="172" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>232</v>
       </c>
@@ -17797,7 +17826,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="173" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>233</v>
       </c>
@@ -17860,7 +17889,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="174" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>234</v>
       </c>
@@ -17923,7 +17952,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="175" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>235</v>
       </c>
@@ -17986,7 +18015,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="176" spans="1:22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>236</v>
       </c>
@@ -18047,7 +18076,7 @@
       <c r="T176"/>
       <c r="U176"/>
     </row>
-    <row r="177" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>237</v>
       </c>
@@ -18110,7 +18139,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>238</v>
       </c>
@@ -18173,7 +18202,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>239</v>
       </c>
@@ -18238,7 +18267,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>240</v>
       </c>
@@ -18303,7 +18332,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>241</v>
       </c>
@@ -18364,7 +18393,7 @@
       <c r="T181"/>
       <c r="U181"/>
     </row>
-    <row r="182" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>242</v>
       </c>
@@ -18427,7 +18456,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>243</v>
       </c>
@@ -18488,7 +18517,7 @@
       <c r="T183"/>
       <c r="U183"/>
     </row>
-    <row r="184" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A184" s="66">
         <v>244</v>
       </c>
@@ -18551,7 +18580,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>245</v>
       </c>
@@ -18612,7 +18641,7 @@
       <c r="T185"/>
       <c r="U185"/>
     </row>
-    <row r="186" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>246</v>
       </c>
@@ -18673,7 +18702,7 @@
       <c r="T186"/>
       <c r="U186"/>
     </row>
-    <row r="187" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>247</v>
       </c>
@@ -18736,7 +18765,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>248</v>
       </c>
@@ -18797,7 +18826,7 @@
       <c r="T188"/>
       <c r="U188"/>
     </row>
-    <row r="189" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>249</v>
       </c>
@@ -18858,7 +18887,7 @@
       <c r="T189"/>
       <c r="U189"/>
     </row>
-    <row r="190" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>250</v>
       </c>
@@ -18919,7 +18948,7 @@
       <c r="T190"/>
       <c r="U190"/>
     </row>
-    <row r="191" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>251</v>
       </c>
@@ -18982,7 +19011,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>252</v>
       </c>
@@ -19043,7 +19072,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>253</v>
       </c>
@@ -19104,7 +19133,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A194" s="68">
         <v>254</v>
       </c>
@@ -19165,7 +19194,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>255</v>
       </c>
@@ -19228,7 +19257,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>256</v>
       </c>
@@ -19291,7 +19320,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>257</v>
       </c>
@@ -19354,7 +19383,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>258</v>
       </c>
@@ -19417,7 +19446,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>259</v>
       </c>
@@ -19480,7 +19509,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>260</v>
       </c>
@@ -19545,7 +19574,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>261</v>
       </c>
@@ -19606,7 +19635,7 @@
       <c r="T201"/>
       <c r="U201"/>
     </row>
-    <row r="202" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>262</v>
       </c>
@@ -19667,7 +19696,7 @@
       <c r="T202"/>
       <c r="U202"/>
     </row>
-    <row r="203" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>263</v>
       </c>
@@ -19728,7 +19757,7 @@
       <c r="T203"/>
       <c r="U203"/>
     </row>
-    <row r="204" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>264</v>
       </c>
@@ -19793,7 +19822,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>265</v>
       </c>
@@ -19858,7 +19887,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>266</v>
       </c>
@@ -19919,7 +19948,7 @@
       <c r="T206"/>
       <c r="U206"/>
     </row>
-    <row r="207" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>267</v>
       </c>
@@ -19982,7 +20011,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>268</v>
       </c>
@@ -20045,7 +20074,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>269</v>
       </c>
@@ -20108,7 +20137,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>270</v>
       </c>
@@ -20171,7 +20200,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A211" s="66">
         <v>271</v>
       </c>
@@ -20234,7 +20263,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>272</v>
       </c>
@@ -20297,7 +20326,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>273</v>
       </c>
@@ -20358,7 +20387,7 @@
       <c r="T213"/>
       <c r="U213"/>
     </row>
-    <row r="214" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>274</v>
       </c>
@@ -20419,7 +20448,7 @@
       <c r="T214"/>
       <c r="U214"/>
     </row>
-    <row r="215" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>275</v>
       </c>
@@ -20482,7 +20511,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>276</v>
       </c>
@@ -20543,7 +20572,7 @@
       <c r="T216"/>
       <c r="U216"/>
     </row>
-    <row r="217" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>277</v>
       </c>
@@ -20606,7 +20635,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>278</v>
       </c>
@@ -20663,7 +20692,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>279</v>
       </c>
@@ -20724,7 +20753,7 @@
       <c r="T219"/>
       <c r="U219"/>
     </row>
-    <row r="220" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>280</v>
       </c>
@@ -20785,7 +20814,7 @@
       <c r="T220"/>
       <c r="U220"/>
     </row>
-    <row r="221" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>281</v>
       </c>
@@ -20846,7 +20875,7 @@
       <c r="T221"/>
       <c r="U221"/>
     </row>
-    <row r="222" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>282</v>
       </c>
@@ -20907,7 +20936,7 @@
       <c r="T222"/>
       <c r="U222"/>
     </row>
-    <row r="223" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A223" s="66">
         <v>283</v>
       </c>
@@ -20970,7 +20999,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>284</v>
       </c>
@@ -21031,7 +21060,7 @@
       <c r="T224"/>
       <c r="U224"/>
     </row>
-    <row r="225" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>285</v>
       </c>
@@ -21092,7 +21121,7 @@
       <c r="T225"/>
       <c r="U225"/>
     </row>
-    <row r="226" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>286</v>
       </c>
@@ -21153,7 +21182,7 @@
       <c r="T226"/>
       <c r="U226"/>
     </row>
-    <row r="227" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>287</v>
       </c>
@@ -21214,7 +21243,7 @@
       <c r="T227"/>
       <c r="U227"/>
     </row>
-    <row r="228" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>288</v>
       </c>
@@ -21275,7 +21304,7 @@
       <c r="T228"/>
       <c r="U228"/>
     </row>
-    <row r="229" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>289</v>
       </c>
@@ -21336,7 +21365,7 @@
       <c r="T229"/>
       <c r="U229"/>
     </row>
-    <row r="230" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>290</v>
       </c>
@@ -21397,7 +21426,7 @@
       <c r="T230"/>
       <c r="U230"/>
     </row>
-    <row r="231" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>291</v>
       </c>
@@ -21460,7 +21489,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>292</v>
       </c>
@@ -21521,7 +21550,7 @@
       <c r="T232"/>
       <c r="U232"/>
     </row>
-    <row r="233" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>293</v>
       </c>
@@ -21582,7 +21611,7 @@
       <c r="T233"/>
       <c r="U233"/>
     </row>
-    <row r="234" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>294</v>
       </c>
@@ -21645,7 +21674,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>295</v>
       </c>
@@ -21708,7 +21737,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>296</v>
       </c>
@@ -21771,7 +21800,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>297</v>
       </c>
@@ -21832,7 +21861,7 @@
       <c r="T237"/>
       <c r="U237"/>
     </row>
-    <row r="238" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>298</v>
       </c>
@@ -21895,7 +21924,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>299</v>
       </c>
@@ -21956,7 +21985,7 @@
       <c r="T239"/>
       <c r="U239"/>
     </row>
-    <row r="240" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>300</v>
       </c>
@@ -22017,7 +22046,7 @@
       <c r="T240"/>
       <c r="U240"/>
     </row>
-    <row r="241" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>301</v>
       </c>
@@ -22080,7 +22109,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>302</v>
       </c>
@@ -22145,7 +22174,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>303</v>
       </c>
@@ -22210,7 +22239,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>304</v>
       </c>
@@ -22275,7 +22304,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>305</v>
       </c>
@@ -22338,7 +22367,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>306</v>
       </c>
@@ -22403,7 +22432,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>307</v>
       </c>
@@ -22466,7 +22495,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>308</v>
       </c>
@@ -22529,7 +22558,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>309</v>
       </c>
@@ -22592,7 +22621,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>310</v>
       </c>
@@ -22655,7 +22684,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>311</v>
       </c>
@@ -22716,7 +22745,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>312</v>
       </c>
@@ -22780,7 +22809,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="L1:L252" xr:uid="{32AFE286-8638-404F-9DBC-2F4BDB10044C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T253">
     <sortCondition ref="B65:B253"/>
   </sortState>
@@ -22791,15 +22819,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD75620-6F76-4BA6-A94E-CE93109D006F}">
-  <dimension ref="A1:AT46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AT50"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X49" sqref="X49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="6" width="15.59765625" style="9"/>
     <col min="7" max="7" width="15.59765625" style="55"/>
@@ -22814,7 +22842,7 @@
     <col min="47" max="16384" width="15.59765625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="50" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" s="50" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -22904,7 +22932,7 @@
       <c r="AS1" s="49"/>
       <c r="AT1" s="49"/>
     </row>
-    <row r="2" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
         <v>313</v>
       </c>
@@ -22965,7 +22993,7 @@
       <c r="T2" s="15"/>
       <c r="U2" s="33"/>
     </row>
-    <row r="3" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>314</v>
       </c>
@@ -23026,7 +23054,7 @@
       <c r="T3" s="15"/>
       <c r="U3" s="33"/>
     </row>
-    <row r="4" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>315</v>
       </c>
@@ -23087,7 +23115,7 @@
       <c r="T4" s="15"/>
       <c r="U4" s="33"/>
     </row>
-    <row r="5" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>316</v>
       </c>
@@ -23148,7 +23176,7 @@
       <c r="T5" s="15"/>
       <c r="U5" s="33"/>
     </row>
-    <row r="6" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>317</v>
       </c>
@@ -23209,7 +23237,7 @@
       <c r="T6" s="15"/>
       <c r="U6" s="33"/>
     </row>
-    <row r="7" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>318</v>
       </c>
@@ -23270,7 +23298,7 @@
       <c r="T7" s="15"/>
       <c r="U7" s="33"/>
     </row>
-    <row r="8" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>319</v>
       </c>
@@ -23331,7 +23359,7 @@
       <c r="T8" s="15"/>
       <c r="U8" s="33"/>
     </row>
-    <row r="9" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>320</v>
       </c>
@@ -23392,7 +23420,7 @@
       <c r="T9" s="15"/>
       <c r="U9" s="33"/>
     </row>
-    <row r="10" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>321</v>
       </c>
@@ -23453,7 +23481,7 @@
       <c r="T10" s="15"/>
       <c r="U10" s="33"/>
     </row>
-    <row r="11" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>322</v>
       </c>
@@ -23514,7 +23542,7 @@
       <c r="T11" s="15"/>
       <c r="U11" s="33"/>
     </row>
-    <row r="12" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>323</v>
       </c>
@@ -23575,7 +23603,7 @@
       <c r="T12" s="15"/>
       <c r="U12" s="33"/>
     </row>
-    <row r="13" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>324</v>
       </c>
@@ -23640,7 +23668,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="14" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>325</v>
       </c>
@@ -23701,7 +23729,7 @@
       <c r="T14" s="15"/>
       <c r="U14" s="33"/>
     </row>
-    <row r="15" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>326</v>
       </c>
@@ -23762,7 +23790,7 @@
       <c r="T15" s="15"/>
       <c r="U15" s="33"/>
     </row>
-    <row r="16" spans="1:46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>327</v>
       </c>
@@ -23823,7 +23851,7 @@
       <c r="T16" s="15"/>
       <c r="U16" s="33"/>
     </row>
-    <row r="17" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>328</v>
       </c>
@@ -23887,7 +23915,7 @@
       </c>
       <c r="U17" s="33"/>
     </row>
-    <row r="18" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>329</v>
       </c>
@@ -23946,7 +23974,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>330</v>
       </c>
@@ -24009,7 +24037,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>331</v>
       </c>
@@ -24072,7 +24100,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>332</v>
       </c>
@@ -24135,7 +24163,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>333</v>
       </c>
@@ -24196,7 +24224,7 @@
       <c r="T22" s="15"/>
       <c r="U22" s="33"/>
     </row>
-    <row r="23" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>334</v>
       </c>
@@ -24261,7 +24289,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>335</v>
       </c>
@@ -24324,7 +24352,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>336</v>
       </c>
@@ -24388,7 +24416,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>337</v>
       </c>
@@ -24453,7 +24481,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <f>A26+1</f>
         <v>338</v>
@@ -24517,9 +24545,9 @@
         <v>568</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
-        <f t="shared" ref="A28:A46" si="0">A27+1</f>
+        <f t="shared" ref="A28:A50" si="0">A27+1</f>
         <v>339</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -24582,7 +24610,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <f t="shared" si="0"/>
         <v>340</v>
@@ -24645,7 +24673,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <f t="shared" si="0"/>
         <v>341</v>
@@ -24708,7 +24736,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <f t="shared" si="0"/>
         <v>342</v>
@@ -24771,7 +24799,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <f t="shared" si="0"/>
         <v>343</v>
@@ -24834,7 +24862,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <f t="shared" si="0"/>
         <v>344</v>
@@ -24897,7 +24925,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <f t="shared" si="0"/>
         <v>345</v>
@@ -24960,7 +24988,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <f t="shared" si="0"/>
         <v>346</v>
@@ -25023,7 +25051,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <f t="shared" si="0"/>
         <v>347</v>
@@ -25086,7 +25114,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <f t="shared" si="0"/>
         <v>348</v>
@@ -25149,7 +25177,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <f t="shared" si="0"/>
         <v>349</v>
@@ -25212,7 +25240,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <f t="shared" si="0"/>
         <v>350</v>
@@ -25277,7 +25305,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
         <f t="shared" si="0"/>
         <v>351</v>
@@ -25343,7 +25371,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <f t="shared" si="0"/>
         <v>352</v>
@@ -25404,7 +25432,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <f t="shared" si="0"/>
         <v>353</v>
@@ -25469,7 +25497,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <f t="shared" si="0"/>
         <v>354</v>
@@ -25534,7 +25562,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <f t="shared" si="0"/>
         <v>355</v>
@@ -25601,7 +25629,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <f t="shared" si="0"/>
         <v>356</v>
@@ -25668,7 +25696,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:22" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="37">
         <f t="shared" si="0"/>
         <v>357</v>
@@ -25734,8 +25762,244 @@
         <v>747</v>
       </c>
     </row>
+    <row r="47" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="69">
+        <f t="shared" si="0"/>
+        <v>358</v>
+      </c>
+      <c r="B47" s="70" t="s">
+        <v>813</v>
+      </c>
+      <c r="C47" s="9">
+        <v>0.83</v>
+      </c>
+      <c r="D47" s="9">
+        <v>1507</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="55">
+        <f>-0.3*61</f>
+        <v>-18.3</v>
+      </c>
+      <c r="H47" s="9">
+        <v>119</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>815</v>
+      </c>
+      <c r="L47" s="9">
+        <v>1293</v>
+      </c>
+      <c r="M47" s="9">
+        <v>-30.510100000000001</v>
+      </c>
+      <c r="N47" s="9">
+        <v>-54.165700000000001</v>
+      </c>
+      <c r="O47" s="9">
+        <v>4</v>
+      </c>
+      <c r="P47" s="9">
+        <v>2011</v>
+      </c>
+      <c r="Q47" s="9">
+        <v>2015</v>
+      </c>
+      <c r="U47" s="8" t="s">
+        <v>816</v>
+      </c>
+      <c r="V47" s="57"/>
+    </row>
+    <row r="48" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="69">
+        <f t="shared" si="0"/>
+        <v>359</v>
+      </c>
+      <c r="B48" s="70" t="s">
+        <v>814</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D48" s="9">
+        <v>1388</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="55">
+        <f>-1*65</f>
+        <v>-65</v>
+      </c>
+      <c r="H48" s="9">
+        <v>348</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>815</v>
+      </c>
+      <c r="L48" s="9">
+        <v>1293</v>
+      </c>
+      <c r="M48" s="9">
+        <v>-30.506900000000002</v>
+      </c>
+      <c r="N48" s="9">
+        <v>-54.167900000000003</v>
+      </c>
+      <c r="O48" s="9">
+        <v>4</v>
+      </c>
+      <c r="P48" s="9">
+        <v>2011</v>
+      </c>
+      <c r="Q48" s="9">
+        <v>2015</v>
+      </c>
+      <c r="U48" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="V48" s="57"/>
+    </row>
+    <row r="49" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="69">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="B49" s="70" t="s">
+        <v>813</v>
+      </c>
+      <c r="C49" s="9">
+        <v>0.83</v>
+      </c>
+      <c r="D49" s="9">
+        <v>2039</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="55">
+        <f>0.3*61</f>
+        <v>18.3</v>
+      </c>
+      <c r="H49" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>812</v>
+      </c>
+      <c r="L49" s="9">
+        <v>1179</v>
+      </c>
+      <c r="M49" s="9">
+        <v>-30.510100000000001</v>
+      </c>
+      <c r="N49" s="9">
+        <v>-54.165700000000001</v>
+      </c>
+      <c r="O49" s="9">
+        <v>4</v>
+      </c>
+      <c r="P49" s="9">
+        <v>2014</v>
+      </c>
+      <c r="Q49" s="9">
+        <v>2018</v>
+      </c>
+      <c r="U49" s="8" t="s">
+        <v>817</v>
+      </c>
+      <c r="V49" s="71"/>
+    </row>
+    <row r="50" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="69">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+      <c r="B50" s="70" t="s">
+        <v>814</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="D50" s="9">
+        <v>2039</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="55">
+        <f>1*65</f>
+        <v>65</v>
+      </c>
+      <c r="H50" s="9">
+        <v>-40</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>812</v>
+      </c>
+      <c r="L50" s="9">
+        <v>1179</v>
+      </c>
+      <c r="M50" s="9">
+        <v>-30.506900000000002</v>
+      </c>
+      <c r="N50" s="9">
+        <v>-54.167900000000003</v>
+      </c>
+      <c r="O50" s="9">
+        <v>4</v>
+      </c>
+      <c r="P50" s="9">
+        <v>2014</v>
+      </c>
+      <c r="Q50" s="9">
+        <v>2018</v>
+      </c>
+      <c r="U50" s="8" t="s">
+        <v>818</v>
+      </c>
+      <c r="V50" s="57"/>
+    </row>
   </sheetData>
-  <autoFilter ref="L1:L46" xr:uid="{4BD75620-6F76-4BA6-A94E-CE93109D006F}"/>
+  <autoFilter ref="L1:L46" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
version ready for resubmission
</commit_message>
<xml_diff>
--- a/data/AllData_Catchments.xlsx
+++ b/data/AllData_Catchments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD489F35-6602-42DE-B87C-9B289892676F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D8179A-21D5-462D-98F1-9FF12ABFA37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LargeCatchments_T1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewCatchments_T3!$L$1:$L$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SmallCatchments_T2!$H$1:$H$252</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2836" uniqueCount="829">
   <si>
     <t>Watershed #</t>
   </si>
@@ -2544,6 +2546,33 @@
   </si>
   <si>
     <t>This should be a decrease in forest cover rather than an increase.</t>
+  </si>
+  <si>
+    <t>Don Tomas</t>
+  </si>
+  <si>
+    <t>Silveira et al., 2016</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>DeltaQf_perc calculated from Table II as (QsNatural grasslands-QsForest/QsNatural grasslands) and yearly averaged</t>
+  </si>
+  <si>
+    <t>La Reina</t>
+  </si>
+  <si>
+    <t>Iroumé A, O Mayen, A Huber. 2006. Runoff and peak flow responses to timber harvest and forest age in southern Chile. Hydrological Processes 20: 37-50. DOI: 10.1002/ hyp.5897</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Andrés Iroumé, Hardin Palacios, Afforestation and changes in forest composition affect runoff in large river basins with pluvial regime and Mediterranean climate, Chile, Journal of Hydrology, Volume 505, 2013, Pages 113-125, ISSN 0022-1694, https://doi.org/10.1016/j.jhydrol.2013.09.031.</t>
+  </si>
+  <si>
+    <t>Iroumé y Palacios., 2013</t>
   </si>
 </sst>
 </file>
@@ -2711,7 +2740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -2883,6 +2912,20 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3199,22 +3242,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="12" width="15.6328125" style="2"/>
-    <col min="13" max="14" width="15.6328125" style="4"/>
-    <col min="15" max="18" width="15.6328125" style="17"/>
-    <col min="19" max="19" width="15.6328125" style="4"/>
-    <col min="21" max="21" width="50.6328125" style="23" customWidth="1"/>
-    <col min="23" max="16384" width="15.6328125" style="2"/>
+    <col min="1" max="12" width="15.59765625" style="2"/>
+    <col min="13" max="14" width="15.59765625" style="4"/>
+    <col min="15" max="18" width="15.59765625" style="17"/>
+    <col min="19" max="19" width="15.59765625" style="4"/>
+    <col min="21" max="21" width="50.59765625" style="23" customWidth="1"/>
+    <col min="23" max="16384" width="15.59765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="8" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="8" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -3279,7 +3322,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3342,7 +3385,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3405,7 +3448,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3468,7 +3511,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3531,7 +3574,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3594,7 +3637,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3655,7 +3698,7 @@
       </c>
       <c r="U7" s="27"/>
     </row>
-    <row r="8" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3716,7 +3759,7 @@
       </c>
       <c r="U8" s="27"/>
     </row>
-    <row r="9" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3777,7 +3820,7 @@
       </c>
       <c r="U9" s="27"/>
     </row>
-    <row r="10" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3840,7 +3883,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3901,7 +3944,7 @@
       </c>
       <c r="U11" s="27"/>
     </row>
-    <row r="12" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3962,7 +4005,7 @@
       </c>
       <c r="U12" s="27"/>
     </row>
-    <row r="13" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4023,7 +4066,7 @@
       </c>
       <c r="U13" s="27"/>
     </row>
-    <row r="14" spans="1:21" s="5" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="5" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>13</v>
       </c>
@@ -4086,7 +4129,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4147,7 +4190,7 @@
       </c>
       <c r="U15" s="27"/>
     </row>
-    <row r="16" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4210,7 +4253,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4272,7 +4315,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4335,7 +4378,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4396,7 +4439,7 @@
       </c>
       <c r="U19" s="27"/>
     </row>
-    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4457,7 +4500,7 @@
       </c>
       <c r="U20" s="27"/>
     </row>
-    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4518,7 +4561,7 @@
       </c>
       <c r="U21" s="27"/>
     </row>
-    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4581,7 +4624,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4644,7 +4687,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4707,7 +4750,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4769,7 +4812,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4832,7 +4875,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4891,7 +4934,7 @@
       </c>
       <c r="U27" s="27"/>
     </row>
-    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4954,7 +4997,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5013,7 +5056,7 @@
       </c>
       <c r="U29" s="27"/>
     </row>
-    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5074,7 +5117,7 @@
       </c>
       <c r="U30" s="27"/>
     </row>
-    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5135,7 +5178,7 @@
       </c>
       <c r="U31" s="27"/>
     </row>
-    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5196,7 +5239,7 @@
       </c>
       <c r="U32" s="27"/>
     </row>
-    <row r="33" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5259,7 +5302,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5320,7 +5363,7 @@
       </c>
       <c r="U34" s="27"/>
     </row>
-    <row r="35" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5379,7 +5422,7 @@
       </c>
       <c r="U35" s="27"/>
     </row>
-    <row r="36" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5438,7 +5481,7 @@
       </c>
       <c r="U36" s="27"/>
     </row>
-    <row r="37" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5499,7 +5542,7 @@
       </c>
       <c r="U37" s="27"/>
     </row>
-    <row r="38" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5559,7 +5602,7 @@
       </c>
       <c r="U38" s="27"/>
     </row>
-    <row r="39" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5620,7 +5663,7 @@
       </c>
       <c r="U39" s="27"/>
     </row>
-    <row r="40" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -5681,7 +5724,7 @@
       </c>
       <c r="U40" s="27"/>
     </row>
-    <row r="41" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -5742,7 +5785,7 @@
       </c>
       <c r="U41" s="27"/>
     </row>
-    <row r="42" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -5805,7 +5848,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -5868,7 +5911,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -5930,7 +5973,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -5992,7 +6035,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -6052,7 +6095,7 @@
       </c>
       <c r="U46" s="27"/>
     </row>
-    <row r="47" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -6115,7 +6158,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -6177,7 +6220,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -6240,7 +6283,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -6301,7 +6344,7 @@
       </c>
       <c r="U50" s="27"/>
     </row>
-    <row r="51" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -6364,7 +6407,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -6427,7 +6470,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -6488,7 +6531,7 @@
       </c>
       <c r="U53" s="27"/>
     </row>
-    <row r="54" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -6547,7 +6590,7 @@
       </c>
       <c r="U54" s="27"/>
     </row>
-    <row r="55" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -6610,7 +6653,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -6671,7 +6714,7 @@
       </c>
       <c r="U56" s="27"/>
     </row>
-    <row r="57" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -6732,7 +6775,7 @@
       </c>
       <c r="U57" s="27"/>
     </row>
-    <row r="58" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -6791,7 +6834,7 @@
       </c>
       <c r="U58" s="27"/>
     </row>
-    <row r="59" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -6852,7 +6895,7 @@
       </c>
       <c r="U59" s="27"/>
     </row>
-    <row r="60" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -6912,7 +6955,7 @@
       </c>
       <c r="U60" s="27"/>
     </row>
-    <row r="61" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -6975,7 +7018,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="21">
         <v>61</v>
       </c>
@@ -7038,7 +7081,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>759</v>
       </c>
@@ -7059,22 +7102,22 @@
       <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="10" width="15.6328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6328125" style="15" customWidth="1"/>
-    <col min="13" max="14" width="15.6328125" style="9" customWidth="1"/>
-    <col min="15" max="17" width="15.6328125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="15.6328125" style="16" customWidth="1"/>
-    <col min="19" max="19" width="15.6328125" style="9" customWidth="1"/>
-    <col min="20" max="20" width="15.6328125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="50.6328125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="10.6328125" style="31"/>
-    <col min="23" max="16384" width="10.6328125" style="10"/>
+    <col min="1" max="10" width="15.59765625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.59765625" style="15" customWidth="1"/>
+    <col min="13" max="14" width="15.59765625" style="9" customWidth="1"/>
+    <col min="15" max="17" width="15.59765625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="15.59765625" style="16" customWidth="1"/>
+    <col min="19" max="19" width="15.59765625" style="9" customWidth="1"/>
+    <col min="20" max="20" width="15.59765625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="50.59765625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="10.59765625" style="31"/>
+    <col min="23" max="16384" width="10.59765625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="39" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="39" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7140,7 +7183,7 @@
       </c>
       <c r="V1" s="30"/>
     </row>
-    <row r="2" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>62</v>
       </c>
@@ -7204,7 +7247,7 @@
       </c>
       <c r="V2" s="31"/>
     </row>
-    <row r="3" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>63</v>
       </c>
@@ -7268,7 +7311,7 @@
       </c>
       <c r="V3" s="31"/>
     </row>
-    <row r="4" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>64</v>
       </c>
@@ -7330,7 +7373,7 @@
       <c r="U4"/>
       <c r="V4" s="31"/>
     </row>
-    <row r="5" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>65</v>
       </c>
@@ -7392,7 +7435,7 @@
       <c r="U5"/>
       <c r="V5" s="31"/>
     </row>
-    <row r="6" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>66</v>
       </c>
@@ -7454,7 +7497,7 @@
       <c r="U6"/>
       <c r="V6" s="31"/>
     </row>
-    <row r="7" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>67</v>
       </c>
@@ -7518,7 +7561,7 @@
       </c>
       <c r="V7" s="31"/>
     </row>
-    <row r="8" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" s="40" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>68</v>
       </c>
@@ -7582,7 +7625,7 @@
       </c>
       <c r="V8" s="31"/>
     </row>
-    <row r="9" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>69</v>
       </c>
@@ -7645,7 +7688,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>70</v>
       </c>
@@ -7708,7 +7751,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>71</v>
       </c>
@@ -7771,7 +7814,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>72</v>
       </c>
@@ -7834,7 +7877,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="66">
         <v>73</v>
       </c>
@@ -7897,7 +7940,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>74</v>
       </c>
@@ -7960,7 +8003,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>75</v>
       </c>
@@ -8023,7 +8066,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>76</v>
       </c>
@@ -8086,7 +8129,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>77</v>
       </c>
@@ -8149,7 +8192,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>78</v>
       </c>
@@ -8212,7 +8255,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>79</v>
       </c>
@@ -8275,7 +8318,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>80</v>
       </c>
@@ -8338,7 +8381,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>81</v>
       </c>
@@ -8401,7 +8444,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>82</v>
       </c>
@@ -8464,7 +8507,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>83</v>
       </c>
@@ -8527,7 +8570,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>84</v>
       </c>
@@ -8588,7 +8631,7 @@
       <c r="T24"/>
       <c r="U24"/>
     </row>
-    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>85</v>
       </c>
@@ -8653,7 +8696,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>86</v>
       </c>
@@ -8716,7 +8759,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>87</v>
       </c>
@@ -8779,7 +8822,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>88</v>
       </c>
@@ -8842,7 +8885,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="66">
         <v>89</v>
       </c>
@@ -8905,7 +8948,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>90</v>
       </c>
@@ -8968,7 +9011,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>91</v>
       </c>
@@ -9029,7 +9072,7 @@
       <c r="T31"/>
       <c r="U31"/>
     </row>
-    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>92</v>
       </c>
@@ -9092,7 +9135,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>93</v>
       </c>
@@ -9157,7 +9200,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>94</v>
       </c>
@@ -9220,7 +9263,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>95</v>
       </c>
@@ -9283,7 +9326,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>96</v>
       </c>
@@ -9344,7 +9387,7 @@
       <c r="T36"/>
       <c r="U36"/>
     </row>
-    <row r="37" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="66">
         <v>97</v>
       </c>
@@ -9407,7 +9450,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>98</v>
       </c>
@@ -9468,7 +9511,7 @@
       <c r="T38"/>
       <c r="U38"/>
     </row>
-    <row r="39" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>99</v>
       </c>
@@ -9529,7 +9572,7 @@
       <c r="T39"/>
       <c r="U39"/>
     </row>
-    <row r="40" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>100</v>
       </c>
@@ -9592,7 +9635,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>101</v>
       </c>
@@ -9653,7 +9696,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>102</v>
       </c>
@@ -9716,7 +9759,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>103</v>
       </c>
@@ -9779,7 +9822,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>104</v>
       </c>
@@ -9842,7 +9885,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>105</v>
       </c>
@@ -9905,7 +9948,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>106</v>
       </c>
@@ -9968,7 +10011,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>107</v>
       </c>
@@ -10031,7 +10074,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>108</v>
       </c>
@@ -10094,7 +10137,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>109</v>
       </c>
@@ -10157,7 +10200,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>110</v>
       </c>
@@ -10220,7 +10263,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>111</v>
       </c>
@@ -10283,7 +10326,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>112</v>
       </c>
@@ -10346,7 +10389,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>113</v>
       </c>
@@ -10409,7 +10452,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>114</v>
       </c>
@@ -10472,7 +10515,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>115</v>
       </c>
@@ -10535,7 +10578,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>116</v>
       </c>
@@ -10598,7 +10641,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>117</v>
       </c>
@@ -10661,7 +10704,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>118</v>
       </c>
@@ -10724,7 +10767,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>119</v>
       </c>
@@ -10785,7 +10828,7 @@
       <c r="T59"/>
       <c r="U59"/>
     </row>
-    <row r="60" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>120</v>
       </c>
@@ -10848,7 +10891,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>121</v>
       </c>
@@ -10911,7 +10954,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>122</v>
       </c>
@@ -10972,7 +11015,7 @@
       <c r="T62"/>
       <c r="U62"/>
     </row>
-    <row r="63" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="66">
         <v>123</v>
       </c>
@@ -11035,7 +11078,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>124</v>
       </c>
@@ -11098,7 +11141,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>125</v>
       </c>
@@ -11159,7 +11202,7 @@
       <c r="T65"/>
       <c r="U65"/>
     </row>
-    <row r="66" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>126</v>
       </c>
@@ -11220,7 +11263,7 @@
       <c r="T66"/>
       <c r="U66"/>
     </row>
-    <row r="67" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>127</v>
       </c>
@@ -11283,7 +11326,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>128</v>
       </c>
@@ -11346,7 +11389,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>129</v>
       </c>
@@ -11409,7 +11452,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>130</v>
       </c>
@@ -11472,7 +11515,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>131</v>
       </c>
@@ -11535,7 +11578,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="66">
         <v>132</v>
       </c>
@@ -11598,7 +11641,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>133</v>
       </c>
@@ -11659,7 +11702,7 @@
       <c r="T73"/>
       <c r="U73"/>
     </row>
-    <row r="74" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>134</v>
       </c>
@@ -11724,7 +11767,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>135</v>
       </c>
@@ -11785,7 +11828,7 @@
       <c r="T75"/>
       <c r="U75"/>
     </row>
-    <row r="76" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>136</v>
       </c>
@@ -11846,7 +11889,7 @@
       <c r="T76"/>
       <c r="U76"/>
     </row>
-    <row r="77" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>137</v>
       </c>
@@ -11909,7 +11952,7 @@
       </c>
       <c r="U77"/>
     </row>
-    <row r="78" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>138</v>
       </c>
@@ -11970,7 +12013,7 @@
       <c r="T78"/>
       <c r="U78"/>
     </row>
-    <row r="79" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>139</v>
       </c>
@@ -12033,7 +12076,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>140</v>
       </c>
@@ -12094,7 +12137,7 @@
       <c r="T80"/>
       <c r="U80"/>
     </row>
-    <row r="81" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>141</v>
       </c>
@@ -12155,7 +12198,7 @@
       <c r="T81"/>
       <c r="U81"/>
     </row>
-    <row r="82" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>142</v>
       </c>
@@ -12218,7 +12261,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>143</v>
       </c>
@@ -12279,7 +12322,7 @@
       <c r="T83"/>
       <c r="U83"/>
     </row>
-    <row r="84" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>144</v>
       </c>
@@ -12342,7 +12385,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>145</v>
       </c>
@@ -12407,7 +12450,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>146</v>
       </c>
@@ -12472,7 +12515,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>147</v>
       </c>
@@ -12535,7 +12578,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>148</v>
       </c>
@@ -12598,7 +12641,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>149</v>
       </c>
@@ -12661,7 +12704,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>150</v>
       </c>
@@ -12724,7 +12767,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>151</v>
       </c>
@@ -12789,7 +12832,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>152</v>
       </c>
@@ -12854,7 +12897,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>153</v>
       </c>
@@ -12919,7 +12962,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>154</v>
       </c>
@@ -12982,7 +13025,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>155</v>
       </c>
@@ -13045,7 +13088,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>156</v>
       </c>
@@ -13110,7 +13153,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>157</v>
       </c>
@@ -13175,7 +13218,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="98" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>158</v>
       </c>
@@ -13233,7 +13276,7 @@
       </c>
       <c r="V98" s="31"/>
     </row>
-    <row r="99" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>159</v>
       </c>
@@ -13298,7 +13341,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="100" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>160</v>
       </c>
@@ -13363,7 +13406,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="66">
         <v>161</v>
       </c>
@@ -13426,7 +13469,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="66">
         <v>162</v>
       </c>
@@ -13489,7 +13532,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="103" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="66">
         <v>163</v>
       </c>
@@ -13552,7 +13595,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>164</v>
       </c>
@@ -13615,7 +13658,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="105" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>165</v>
       </c>
@@ -13680,7 +13723,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="106" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>166</v>
       </c>
@@ -13743,7 +13786,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>167</v>
       </c>
@@ -13804,7 +13847,7 @@
       <c r="T107"/>
       <c r="U107"/>
     </row>
-    <row r="108" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>168</v>
       </c>
@@ -13867,7 +13910,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="109" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>169</v>
       </c>
@@ -13928,7 +13971,7 @@
       <c r="T109"/>
       <c r="U109"/>
     </row>
-    <row r="110" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>170</v>
       </c>
@@ -13991,7 +14034,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="111" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>171</v>
       </c>
@@ -14052,7 +14095,7 @@
       <c r="T111"/>
       <c r="U111"/>
     </row>
-    <row r="112" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>172</v>
       </c>
@@ -14114,7 +14157,7 @@
       <c r="U112"/>
       <c r="V112" s="31"/>
     </row>
-    <row r="113" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>173</v>
       </c>
@@ -14175,7 +14218,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="114" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>174</v>
       </c>
@@ -14236,7 +14279,7 @@
       <c r="T114"/>
       <c r="U114"/>
     </row>
-    <row r="115" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>175</v>
       </c>
@@ -14300,7 +14343,7 @@
       </c>
       <c r="V115" s="31"/>
     </row>
-    <row r="116" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>176</v>
       </c>
@@ -14363,7 +14406,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="117" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>177</v>
       </c>
@@ -14426,7 +14469,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="118" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>178</v>
       </c>
@@ -14488,7 +14531,7 @@
       <c r="U118"/>
       <c r="V118" s="31"/>
     </row>
-    <row r="119" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>179</v>
       </c>
@@ -14551,7 +14594,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="120" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>180</v>
       </c>
@@ -14614,7 +14657,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="121" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A121" s="66">
         <v>181</v>
       </c>
@@ -14677,7 +14720,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="122" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>182</v>
       </c>
@@ -14738,7 +14781,7 @@
       <c r="T122"/>
       <c r="U122"/>
     </row>
-    <row r="123" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>183</v>
       </c>
@@ -14799,7 +14842,7 @@
       <c r="T123"/>
       <c r="U123"/>
     </row>
-    <row r="124" spans="1:22" s="13" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:22" s="13" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>184</v>
       </c>
@@ -14865,7 +14908,7 @@
       </c>
       <c r="V124" s="31"/>
     </row>
-    <row r="125" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>185</v>
       </c>
@@ -14915,7 +14958,7 @@
       </c>
       <c r="V125" s="31"/>
     </row>
-    <row r="126" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>186</v>
       </c>
@@ -14976,7 +15019,7 @@
       <c r="T126"/>
       <c r="U126"/>
     </row>
-    <row r="127" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>187</v>
       </c>
@@ -15039,7 +15082,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="128" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A128" s="68">
         <v>188</v>
       </c>
@@ -15100,7 +15143,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="129" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>189</v>
       </c>
@@ -15160,7 +15203,7 @@
       </c>
       <c r="V129" s="31"/>
     </row>
-    <row r="130" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>190</v>
       </c>
@@ -15221,7 +15264,7 @@
       <c r="T130"/>
       <c r="U130"/>
     </row>
-    <row r="131" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>191</v>
       </c>
@@ -15284,7 +15327,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="132" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>192</v>
       </c>
@@ -15347,7 +15390,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="133" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>193</v>
       </c>
@@ -15408,7 +15451,7 @@
       <c r="T133"/>
       <c r="U133"/>
     </row>
-    <row r="134" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>194</v>
       </c>
@@ -15471,7 +15514,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="135" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>195</v>
       </c>
@@ -15534,7 +15577,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="136" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>196</v>
       </c>
@@ -15597,7 +15640,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="137" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:22" s="12" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>197</v>
       </c>
@@ -15647,7 +15690,7 @@
       </c>
       <c r="V137" s="31"/>
     </row>
-    <row r="138" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>198</v>
       </c>
@@ -15708,7 +15751,7 @@
       <c r="T138"/>
       <c r="U138"/>
     </row>
-    <row r="139" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>199</v>
       </c>
@@ -15771,7 +15814,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="140" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>200</v>
       </c>
@@ -15832,7 +15875,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="141" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>201</v>
       </c>
@@ -15891,7 +15934,7 @@
       <c r="T141"/>
       <c r="U141"/>
     </row>
-    <row r="142" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>202</v>
       </c>
@@ -15952,7 +15995,7 @@
       <c r="T142"/>
       <c r="U142"/>
     </row>
-    <row r="143" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>203</v>
       </c>
@@ -16015,7 +16058,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="144" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>204</v>
       </c>
@@ -16078,7 +16121,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>205</v>
       </c>
@@ -16139,7 +16182,7 @@
       <c r="T145"/>
       <c r="U145"/>
     </row>
-    <row r="146" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>206</v>
       </c>
@@ -16200,7 +16243,7 @@
       <c r="T146"/>
       <c r="U146"/>
     </row>
-    <row r="147" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>207</v>
       </c>
@@ -16263,7 +16306,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>208</v>
       </c>
@@ -16326,7 +16369,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>209</v>
       </c>
@@ -16389,7 +16432,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>210</v>
       </c>
@@ -16452,7 +16495,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>211</v>
       </c>
@@ -16513,7 +16556,7 @@
       <c r="T151"/>
       <c r="U151"/>
     </row>
-    <row r="152" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>212</v>
       </c>
@@ -16574,7 +16617,7 @@
       <c r="T152"/>
       <c r="U152"/>
     </row>
-    <row r="153" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>213</v>
       </c>
@@ -16637,7 +16680,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>214</v>
       </c>
@@ -16700,7 +16743,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>215</v>
       </c>
@@ -16763,7 +16806,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>216</v>
       </c>
@@ -16824,7 +16867,7 @@
       <c r="T156"/>
       <c r="U156"/>
     </row>
-    <row r="157" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>217</v>
       </c>
@@ -16885,7 +16928,7 @@
       <c r="T157"/>
       <c r="U157"/>
     </row>
-    <row r="158" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>218</v>
       </c>
@@ -16946,7 +16989,7 @@
       <c r="T158"/>
       <c r="U158"/>
     </row>
-    <row r="159" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>219</v>
       </c>
@@ -17009,7 +17052,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>220</v>
       </c>
@@ -17074,7 +17117,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>221</v>
       </c>
@@ -17137,7 +17180,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="162" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>222</v>
       </c>
@@ -17200,7 +17243,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="163" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>223</v>
       </c>
@@ -17265,7 +17308,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="164" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>224</v>
       </c>
@@ -17328,7 +17371,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="165" spans="1:22" s="11" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:22" s="11" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>225</v>
       </c>
@@ -17392,7 +17435,7 @@
       </c>
       <c r="V165" s="31"/>
     </row>
-    <row r="166" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>226</v>
       </c>
@@ -17453,7 +17496,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="167" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>227</v>
       </c>
@@ -17518,7 +17561,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>228</v>
       </c>
@@ -17579,7 +17622,7 @@
       <c r="T168"/>
       <c r="U168"/>
     </row>
-    <row r="169" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>229</v>
       </c>
@@ -17640,7 +17683,7 @@
       <c r="T169"/>
       <c r="U169"/>
     </row>
-    <row r="170" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>230</v>
       </c>
@@ -17701,7 +17744,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>231</v>
       </c>
@@ -17764,7 +17807,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="172" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>232</v>
       </c>
@@ -17827,7 +17870,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="173" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>233</v>
       </c>
@@ -17890,7 +17933,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="174" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>234</v>
       </c>
@@ -17953,7 +17996,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="175" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>235</v>
       </c>
@@ -18016,7 +18059,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="176" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>236</v>
       </c>
@@ -18077,7 +18120,7 @@
       <c r="T176"/>
       <c r="U176"/>
     </row>
-    <row r="177" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>237</v>
       </c>
@@ -18140,7 +18183,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>238</v>
       </c>
@@ -18203,7 +18246,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>239</v>
       </c>
@@ -18268,7 +18311,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>240</v>
       </c>
@@ -18333,7 +18376,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>241</v>
       </c>
@@ -18394,7 +18437,7 @@
       <c r="T181"/>
       <c r="U181"/>
     </row>
-    <row r="182" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>242</v>
       </c>
@@ -18457,7 +18500,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>243</v>
       </c>
@@ -18518,7 +18561,7 @@
       <c r="T183"/>
       <c r="U183"/>
     </row>
-    <row r="184" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A184" s="66">
         <v>244</v>
       </c>
@@ -18581,7 +18624,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>245</v>
       </c>
@@ -18642,7 +18685,7 @@
       <c r="T185"/>
       <c r="U185"/>
     </row>
-    <row r="186" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>246</v>
       </c>
@@ -18703,7 +18746,7 @@
       <c r="T186"/>
       <c r="U186"/>
     </row>
-    <row r="187" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>247</v>
       </c>
@@ -18766,7 +18809,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>248</v>
       </c>
@@ -18827,7 +18870,7 @@
       <c r="T188"/>
       <c r="U188"/>
     </row>
-    <row r="189" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>249</v>
       </c>
@@ -18888,7 +18931,7 @@
       <c r="T189"/>
       <c r="U189"/>
     </row>
-    <row r="190" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>250</v>
       </c>
@@ -18949,7 +18992,7 @@
       <c r="T190"/>
       <c r="U190"/>
     </row>
-    <row r="191" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>251</v>
       </c>
@@ -19012,7 +19055,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>252</v>
       </c>
@@ -19073,7 +19116,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>253</v>
       </c>
@@ -19134,7 +19177,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A194" s="68">
         <v>254</v>
       </c>
@@ -19195,7 +19238,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>255</v>
       </c>
@@ -19258,7 +19301,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>256</v>
       </c>
@@ -19321,7 +19364,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>257</v>
       </c>
@@ -19384,7 +19427,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>258</v>
       </c>
@@ -19447,7 +19490,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>259</v>
       </c>
@@ -19510,7 +19553,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>260</v>
       </c>
@@ -19575,7 +19618,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>261</v>
       </c>
@@ -19636,7 +19679,7 @@
       <c r="T201"/>
       <c r="U201"/>
     </row>
-    <row r="202" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>262</v>
       </c>
@@ -19697,7 +19740,7 @@
       <c r="T202"/>
       <c r="U202"/>
     </row>
-    <row r="203" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>263</v>
       </c>
@@ -19758,7 +19801,7 @@
       <c r="T203"/>
       <c r="U203"/>
     </row>
-    <row r="204" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>264</v>
       </c>
@@ -19823,7 +19866,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>265</v>
       </c>
@@ -19888,7 +19931,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>266</v>
       </c>
@@ -19949,7 +19992,7 @@
       <c r="T206"/>
       <c r="U206"/>
     </row>
-    <row r="207" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>267</v>
       </c>
@@ -20012,7 +20055,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>268</v>
       </c>
@@ -20075,7 +20118,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>269</v>
       </c>
@@ -20138,7 +20181,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>270</v>
       </c>
@@ -20201,7 +20244,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A211" s="66">
         <v>271</v>
       </c>
@@ -20264,7 +20307,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>272</v>
       </c>
@@ -20327,7 +20370,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>273</v>
       </c>
@@ -20388,7 +20431,7 @@
       <c r="T213"/>
       <c r="U213"/>
     </row>
-    <row r="214" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>274</v>
       </c>
@@ -20449,7 +20492,7 @@
       <c r="T214"/>
       <c r="U214"/>
     </row>
-    <row r="215" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>275</v>
       </c>
@@ -20512,7 +20555,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>276</v>
       </c>
@@ -20573,7 +20616,7 @@
       <c r="T216"/>
       <c r="U216"/>
     </row>
-    <row r="217" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>277</v>
       </c>
@@ -20636,7 +20679,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>278</v>
       </c>
@@ -20693,7 +20736,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>279</v>
       </c>
@@ -20754,7 +20797,7 @@
       <c r="T219"/>
       <c r="U219"/>
     </row>
-    <row r="220" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>280</v>
       </c>
@@ -20815,7 +20858,7 @@
       <c r="T220"/>
       <c r="U220"/>
     </row>
-    <row r="221" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>281</v>
       </c>
@@ -20876,7 +20919,7 @@
       <c r="T221"/>
       <c r="U221"/>
     </row>
-    <row r="222" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>282</v>
       </c>
@@ -20937,7 +20980,7 @@
       <c r="T222"/>
       <c r="U222"/>
     </row>
-    <row r="223" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A223" s="66">
         <v>283</v>
       </c>
@@ -21000,7 +21043,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>284</v>
       </c>
@@ -21061,7 +21104,7 @@
       <c r="T224"/>
       <c r="U224"/>
     </row>
-    <row r="225" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>285</v>
       </c>
@@ -21122,7 +21165,7 @@
       <c r="T225"/>
       <c r="U225"/>
     </row>
-    <row r="226" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>286</v>
       </c>
@@ -21183,7 +21226,7 @@
       <c r="T226"/>
       <c r="U226"/>
     </row>
-    <row r="227" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>287</v>
       </c>
@@ -21244,7 +21287,7 @@
       <c r="T227"/>
       <c r="U227"/>
     </row>
-    <row r="228" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>288</v>
       </c>
@@ -21305,7 +21348,7 @@
       <c r="T228"/>
       <c r="U228"/>
     </row>
-    <row r="229" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>289</v>
       </c>
@@ -21366,7 +21409,7 @@
       <c r="T229"/>
       <c r="U229"/>
     </row>
-    <row r="230" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>290</v>
       </c>
@@ -21427,7 +21470,7 @@
       <c r="T230"/>
       <c r="U230"/>
     </row>
-    <row r="231" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>291</v>
       </c>
@@ -21490,7 +21533,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>292</v>
       </c>
@@ -21551,7 +21594,7 @@
       <c r="T232"/>
       <c r="U232"/>
     </row>
-    <row r="233" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>293</v>
       </c>
@@ -21612,7 +21655,7 @@
       <c r="T233"/>
       <c r="U233"/>
     </row>
-    <row r="234" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>294</v>
       </c>
@@ -21675,7 +21718,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>295</v>
       </c>
@@ -21738,7 +21781,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>296</v>
       </c>
@@ -21801,7 +21844,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>297</v>
       </c>
@@ -21862,7 +21905,7 @@
       <c r="T237"/>
       <c r="U237"/>
     </row>
-    <row r="238" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>298</v>
       </c>
@@ -21925,7 +21968,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>299</v>
       </c>
@@ -21986,7 +22029,7 @@
       <c r="T239"/>
       <c r="U239"/>
     </row>
-    <row r="240" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>300</v>
       </c>
@@ -22047,7 +22090,7 @@
       <c r="T240"/>
       <c r="U240"/>
     </row>
-    <row r="241" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>301</v>
       </c>
@@ -22110,7 +22153,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>302</v>
       </c>
@@ -22175,7 +22218,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>303</v>
       </c>
@@ -22240,7 +22283,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>304</v>
       </c>
@@ -22305,7 +22348,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>305</v>
       </c>
@@ -22368,7 +22411,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>306</v>
       </c>
@@ -22433,7 +22476,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>307</v>
       </c>
@@ -22496,7 +22539,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>308</v>
       </c>
@@ -22559,7 +22602,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>309</v>
       </c>
@@ -22622,7 +22665,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>310</v>
       </c>
@@ -22685,7 +22728,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>311</v>
       </c>
@@ -22746,7 +22789,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>312</v>
       </c>
@@ -22821,29 +22864,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AT50"/>
+  <dimension ref="A1:AT55"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X49" sqref="X49"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L52" sqref="L52:L55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.59765625" defaultRowHeight="40.15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="15.6328125" style="9"/>
-    <col min="7" max="7" width="15.6328125" style="55"/>
-    <col min="8" max="9" width="15.6328125" style="9"/>
-    <col min="10" max="10" width="15.6328125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.6328125" style="8"/>
-    <col min="12" max="17" width="15.6328125" style="9"/>
-    <col min="18" max="18" width="15.6328125" style="14"/>
-    <col min="19" max="20" width="15.6328125" style="9"/>
-    <col min="21" max="21" width="50.6328125" style="8" customWidth="1"/>
-    <col min="22" max="46" width="15.6328125" style="15"/>
-    <col min="47" max="16384" width="15.6328125" style="9"/>
+    <col min="1" max="6" width="15.59765625" style="9"/>
+    <col min="7" max="7" width="15.59765625" style="55"/>
+    <col min="8" max="9" width="15.59765625" style="9"/>
+    <col min="10" max="10" width="15.59765625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" style="8"/>
+    <col min="12" max="17" width="15.59765625" style="9"/>
+    <col min="18" max="18" width="15.59765625" style="14"/>
+    <col min="19" max="20" width="15.59765625" style="9"/>
+    <col min="21" max="21" width="50.59765625" style="8" customWidth="1"/>
+    <col min="22" max="46" width="15.59765625" style="15"/>
+    <col min="47" max="16384" width="15.59765625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="50" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="50" customFormat="1" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -22933,7 +22976,7 @@
       <c r="AS1" s="49"/>
       <c r="AT1" s="49"/>
     </row>
-    <row r="2" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
         <v>313</v>
       </c>
@@ -22994,7 +23037,7 @@
       <c r="T2" s="15"/>
       <c r="U2" s="33"/>
     </row>
-    <row r="3" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>314</v>
       </c>
@@ -23055,7 +23098,7 @@
       <c r="T3" s="15"/>
       <c r="U3" s="33"/>
     </row>
-    <row r="4" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>315</v>
       </c>
@@ -23116,7 +23159,7 @@
       <c r="T4" s="15"/>
       <c r="U4" s="33"/>
     </row>
-    <row r="5" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>316</v>
       </c>
@@ -23177,7 +23220,7 @@
       <c r="T5" s="15"/>
       <c r="U5" s="33"/>
     </row>
-    <row r="6" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>317</v>
       </c>
@@ -23238,7 +23281,7 @@
       <c r="T6" s="15"/>
       <c r="U6" s="33"/>
     </row>
-    <row r="7" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>318</v>
       </c>
@@ -23299,7 +23342,7 @@
       <c r="T7" s="15"/>
       <c r="U7" s="33"/>
     </row>
-    <row r="8" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>319</v>
       </c>
@@ -23360,7 +23403,7 @@
       <c r="T8" s="15"/>
       <c r="U8" s="33"/>
     </row>
-    <row r="9" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>320</v>
       </c>
@@ -23421,7 +23464,7 @@
       <c r="T9" s="15"/>
       <c r="U9" s="33"/>
     </row>
-    <row r="10" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>321</v>
       </c>
@@ -23482,7 +23525,7 @@
       <c r="T10" s="15"/>
       <c r="U10" s="33"/>
     </row>
-    <row r="11" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>322</v>
       </c>
@@ -23543,7 +23586,7 @@
       <c r="T11" s="15"/>
       <c r="U11" s="33"/>
     </row>
-    <row r="12" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>323</v>
       </c>
@@ -23604,7 +23647,7 @@
       <c r="T12" s="15"/>
       <c r="U12" s="33"/>
     </row>
-    <row r="13" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>324</v>
       </c>
@@ -23669,7 +23712,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="14" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>325</v>
       </c>
@@ -23730,7 +23773,7 @@
       <c r="T14" s="15"/>
       <c r="U14" s="33"/>
     </row>
-    <row r="15" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>326</v>
       </c>
@@ -23791,7 +23834,7 @@
       <c r="T15" s="15"/>
       <c r="U15" s="33"/>
     </row>
-    <row r="16" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>327</v>
       </c>
@@ -23852,7 +23895,7 @@
       <c r="T16" s="15"/>
       <c r="U16" s="33"/>
     </row>
-    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>328</v>
       </c>
@@ -23916,7 +23959,7 @@
       </c>
       <c r="U17" s="33"/>
     </row>
-    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>329</v>
       </c>
@@ -23975,7 +24018,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>330</v>
       </c>
@@ -24038,7 +24081,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>331</v>
       </c>
@@ -24101,7 +24144,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>332</v>
       </c>
@@ -24164,7 +24207,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>333</v>
       </c>
@@ -24225,7 +24268,7 @@
       <c r="T22" s="15"/>
       <c r="U22" s="33"/>
     </row>
-    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>334</v>
       </c>
@@ -24290,7 +24333,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>335</v>
       </c>
@@ -24353,7 +24396,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>336</v>
       </c>
@@ -24417,7 +24460,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>337</v>
       </c>
@@ -24482,7 +24525,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <f>A26+1</f>
         <v>338</v>
@@ -24546,9 +24589,9 @@
         <v>567</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
-        <f t="shared" ref="A28:A50" si="0">A27+1</f>
+        <f t="shared" ref="A28:A55" si="0">A27+1</f>
         <v>339</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -24611,7 +24654,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <f t="shared" si="0"/>
         <v>340</v>
@@ -24674,7 +24717,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <f t="shared" si="0"/>
         <v>341</v>
@@ -24737,7 +24780,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <f t="shared" si="0"/>
         <v>342</v>
@@ -24800,7 +24843,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <f t="shared" si="0"/>
         <v>343</v>
@@ -24863,7 +24906,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <f t="shared" si="0"/>
         <v>344</v>
@@ -24926,7 +24969,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <f t="shared" si="0"/>
         <v>345</v>
@@ -24989,7 +25032,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <f t="shared" si="0"/>
         <v>346</v>
@@ -25052,7 +25095,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <f t="shared" si="0"/>
         <v>347</v>
@@ -25115,7 +25158,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <f t="shared" si="0"/>
         <v>348</v>
@@ -25178,7 +25221,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <f t="shared" si="0"/>
         <v>349</v>
@@ -25241,7 +25284,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <f t="shared" si="0"/>
         <v>350</v>
@@ -25306,7 +25349,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
         <f t="shared" si="0"/>
         <v>351</v>
@@ -25372,7 +25415,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <f t="shared" si="0"/>
         <v>352</v>
@@ -25433,7 +25476,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <f t="shared" si="0"/>
         <v>353</v>
@@ -25498,7 +25541,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <f t="shared" si="0"/>
         <v>354</v>
@@ -25563,7 +25606,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <f t="shared" si="0"/>
         <v>355</v>
@@ -25630,7 +25673,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <f t="shared" si="0"/>
         <v>356</v>
@@ -25697,7 +25740,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="37">
         <f t="shared" si="0"/>
         <v>357</v>
@@ -25763,7 +25806,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="69">
         <f t="shared" si="0"/>
         <v>358</v>
@@ -25822,7 +25865,7 @@
       </c>
       <c r="V47" s="57"/>
     </row>
-    <row r="48" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="69">
         <f t="shared" si="0"/>
         <v>359</v>
@@ -25881,7 +25924,7 @@
       </c>
       <c r="V48" s="57"/>
     </row>
-    <row r="49" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="69">
         <f t="shared" si="0"/>
         <v>360</v>
@@ -25940,7 +25983,7 @@
       </c>
       <c r="V49" s="71"/>
     </row>
-    <row r="50" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="69">
         <f t="shared" si="0"/>
         <v>361</v>
@@ -25998,6 +26041,318 @@
         <v>815</v>
       </c>
       <c r="V50" s="57"/>
+    </row>
+    <row r="51" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="78">
+        <f t="shared" si="0"/>
+        <v>362</v>
+      </c>
+      <c r="B51" s="79" t="s">
+        <v>820</v>
+      </c>
+      <c r="C51" s="75">
+        <v>2.12</v>
+      </c>
+      <c r="D51" s="75">
+        <v>1468</v>
+      </c>
+      <c r="E51" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="77">
+        <v>56</v>
+      </c>
+      <c r="H51" s="75">
+        <v>-43</v>
+      </c>
+      <c r="I51" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" s="74" t="s">
+        <v>821</v>
+      </c>
+      <c r="L51" s="75">
+        <v>1496</v>
+      </c>
+      <c r="M51" s="75">
+        <v>-32.249000000000002</v>
+      </c>
+      <c r="N51" s="75">
+        <v>-57.646999999999998</v>
+      </c>
+      <c r="O51" s="75">
+        <v>8</v>
+      </c>
+      <c r="P51" s="75">
+        <v>2006</v>
+      </c>
+      <c r="Q51" s="75">
+        <v>2014</v>
+      </c>
+      <c r="R51" s="76" t="s">
+        <v>822</v>
+      </c>
+      <c r="S51" s="75">
+        <v>1</v>
+      </c>
+      <c r="T51" s="73"/>
+      <c r="U51" s="74" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="78">
+        <f t="shared" si="0"/>
+        <v>363</v>
+      </c>
+      <c r="B52" s="79" t="s">
+        <v>824</v>
+      </c>
+      <c r="C52" s="75">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="D52" s="75">
+        <v>2596</v>
+      </c>
+      <c r="E52" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="77">
+        <v>-79.400000000000006</v>
+      </c>
+      <c r="H52" s="75">
+        <v>110</v>
+      </c>
+      <c r="I52" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="74" t="s">
+        <v>825</v>
+      </c>
+      <c r="L52" s="80">
+        <v>1255</v>
+      </c>
+      <c r="M52" s="75">
+        <v>-40.343000000000004</v>
+      </c>
+      <c r="N52" s="75">
+        <v>-73.453000000000003</v>
+      </c>
+      <c r="O52" s="75">
+        <v>6</v>
+      </c>
+      <c r="P52" s="75">
+        <v>1997</v>
+      </c>
+      <c r="Q52" s="75">
+        <v>2002</v>
+      </c>
+      <c r="R52" s="76" t="s">
+        <v>826</v>
+      </c>
+      <c r="S52" s="75">
+        <v>1</v>
+      </c>
+      <c r="T52" s="73"/>
+      <c r="U52" s="73"/>
+    </row>
+    <row r="53" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="78">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+      <c r="B53" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="75">
+        <v>1595</v>
+      </c>
+      <c r="D53" s="75">
+        <v>1660</v>
+      </c>
+      <c r="E53" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="77">
+        <v>15.9</v>
+      </c>
+      <c r="H53" s="75">
+        <v>-22.2</v>
+      </c>
+      <c r="I53" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="K53" s="74" t="s">
+        <v>827</v>
+      </c>
+      <c r="L53" s="80">
+        <v>871</v>
+      </c>
+      <c r="M53" s="75">
+        <v>-37.585000000000001</v>
+      </c>
+      <c r="N53" s="75">
+        <v>-72.147999999999996</v>
+      </c>
+      <c r="O53" s="75">
+        <v>44</v>
+      </c>
+      <c r="P53" s="75">
+        <v>1962</v>
+      </c>
+      <c r="Q53" s="75">
+        <v>2005</v>
+      </c>
+      <c r="R53" s="76" t="s">
+        <v>826</v>
+      </c>
+      <c r="S53" s="75">
+        <v>1</v>
+      </c>
+      <c r="T53" s="73"/>
+      <c r="U53" s="73"/>
+    </row>
+    <row r="54" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="78">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="B54" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" s="75">
+        <v>94</v>
+      </c>
+      <c r="D54" s="75">
+        <v>1170</v>
+      </c>
+      <c r="E54" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="77">
+        <v>18.7</v>
+      </c>
+      <c r="H54" s="75">
+        <v>-6.4</v>
+      </c>
+      <c r="I54" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="K54" s="74" t="s">
+        <v>828</v>
+      </c>
+      <c r="L54" s="80">
+        <v>1188</v>
+      </c>
+      <c r="M54" s="75">
+        <v>-37.68</v>
+      </c>
+      <c r="N54" s="75">
+        <v>-73.23</v>
+      </c>
+      <c r="O54" s="75">
+        <v>31</v>
+      </c>
+      <c r="P54" s="75">
+        <v>1962</v>
+      </c>
+      <c r="Q54" s="75">
+        <v>1992</v>
+      </c>
+      <c r="R54" s="76" t="s">
+        <v>826</v>
+      </c>
+      <c r="S54" s="75">
+        <v>1</v>
+      </c>
+      <c r="T54" s="73"/>
+      <c r="U54" s="73"/>
+    </row>
+    <row r="55" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="78">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="B55" s="79" t="s">
+        <v>347</v>
+      </c>
+      <c r="C55" s="75">
+        <v>434</v>
+      </c>
+      <c r="D55" s="75">
+        <v>1660</v>
+      </c>
+      <c r="E55" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="77">
+        <v>50</v>
+      </c>
+      <c r="H55" s="75">
+        <v>-25.5</v>
+      </c>
+      <c r="I55" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="K55" s="74" t="s">
+        <v>828</v>
+      </c>
+      <c r="L55" s="80">
+        <v>1029</v>
+      </c>
+      <c r="M55" s="75">
+        <v>-37.905000000000001</v>
+      </c>
+      <c r="N55" s="75">
+        <v>-72.033000000000001</v>
+      </c>
+      <c r="O55" s="75">
+        <v>44</v>
+      </c>
+      <c r="P55" s="75">
+        <v>1962</v>
+      </c>
+      <c r="Q55" s="75">
+        <v>2005</v>
+      </c>
+      <c r="R55" s="76" t="s">
+        <v>826</v>
+      </c>
+      <c r="S55" s="75">
+        <v>1</v>
+      </c>
+      <c r="T55" s="73"/>
+      <c r="U55" s="73"/>
     </row>
   </sheetData>
   <autoFilter ref="L1:L46" xr:uid="{00000000-0009-0000-0000-000002000000}"/>

</xml_diff>